<commit_message>
patch meteor and update gantt chart
</commit_message>
<xml_diff>
--- a/documentation/ESAP_Gantt_Chart.xlsx
+++ b/documentation/ESAP_Gantt_Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="2480" windowWidth="32120" windowHeight="20440"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23920"/>
   </bookViews>
   <sheets>
     <sheet name="gantt chart" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="92">
   <si>
     <t>Plan</t>
   </si>
@@ -231,9 +231,6 @@
     <t>MILESTONE</t>
   </si>
   <si>
-    <t>Design Site</t>
-  </si>
-  <si>
     <t>Fill Out Gantt Chart</t>
   </si>
   <si>
@@ -364,6 +361,18 @@
   </si>
   <si>
     <t>Create collection for schools and its methods</t>
+  </si>
+  <si>
+    <t>Update collection schemas</t>
+  </si>
+  <si>
+    <t>Make buildings collection generic for all types</t>
+  </si>
+  <si>
+    <t>Come up with schema for ratings (i.e. what to rate)</t>
+  </si>
+  <si>
+    <t>Design</t>
   </si>
 </sst>
 </file>
@@ -828,7 +837,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -931,6 +940,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="7" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -945,69 +1020,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="7" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="64">
@@ -1254,7 +1266,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="11"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1533,24 +1545,24 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BE70"/>
+  <dimension ref="A2:BE73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="53" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1640625" style="43" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="39" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" style="33" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" style="33" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="33" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="58" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="54" customWidth="1"/>
     <col min="11" max="11" width="2.83203125" style="33" customWidth="1"/>
     <col min="12" max="16" width="3.1640625" style="33" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="3.5" style="33" bestFit="1" customWidth="1"/>
@@ -1570,112 +1582,112 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:57" ht="19" customHeight="1">
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="L2" s="47" t="s">
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="L2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="47"/>
-      <c r="P2" s="47"/>
-      <c r="Q2" s="48">
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
+      <c r="Q2" s="44">
         <f ca="1">DAYS360(P4,today+1)</f>
-        <v>10</v>
-      </c>
-      <c r="R2" s="47"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" s="43"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="51"/>
-      <c r="X2" s="50" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="52"/>
-      <c r="AB2" s="53" t="s">
+      <c r="W2" s="47"/>
+      <c r="X2" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="53" t="s">
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="49" t="s">
         <v>9</v>
       </c>
       <c r="AJ2" s="33"/>
       <c r="AK2" s="33"/>
       <c r="AL2" s="33"/>
       <c r="AM2" s="33"/>
-      <c r="AN2" s="55"/>
-      <c r="AO2" s="53" t="s">
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="49" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:57" ht="27" customHeight="1">
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35"/>
-      <c r="I3" s="46"/>
-      <c r="J3" s="46"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="42"/>
+      <c r="J3" s="42"/>
     </row>
     <row r="4" spans="1:57" ht="18.75" customHeight="1">
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="58" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="46"/>
-      <c r="J4" s="46"/>
-      <c r="L4" s="38" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="58"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="58"/>
+      <c r="H4" s="58"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="L4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="38"/>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="37">
+      <c r="M4" s="60"/>
+      <c r="N4" s="60"/>
+      <c r="O4" s="60"/>
+      <c r="P4" s="59">
         <v>42660</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
       <c r="T4" s="1"/>
-      <c r="AA4" s="38" t="s">
+      <c r="AA4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="38"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="38"/>
-      <c r="AE4" s="37">
+      <c r="AB4" s="60"/>
+      <c r="AC4" s="60"/>
+      <c r="AD4" s="60"/>
+      <c r="AE4" s="59">
         <v>42688</v>
       </c>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="38"/>
-      <c r="AH4" s="38"/>
+      <c r="AF4" s="60"/>
+      <c r="AG4" s="60"/>
+      <c r="AH4" s="60"/>
       <c r="AI4" s="33"/>
       <c r="AJ4" s="33"/>
       <c r="AK4" s="33"/>
-      <c r="AN4" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="AR4" s="34">
+      <c r="AN4" s="52" t="s">
+        <v>48</v>
+      </c>
+      <c r="AR4" s="56">
         <f ca="1">TODAY()</f>
-        <v>42669</v>
-      </c>
-      <c r="AS4" s="34"/>
-      <c r="AT4" s="34"/>
-      <c r="AU4" s="34"/>
+        <v>42670</v>
+      </c>
+      <c r="AS4" s="56"/>
+      <c r="AT4" s="56"/>
+      <c r="AU4" s="56"/>
       <c r="AW4" s="33"/>
       <c r="AX4" s="33"/>
       <c r="AY4" s="33"/>
@@ -1684,42 +1696,42 @@
     </row>
     <row r="5" spans="1:57">
       <c r="G5" s="1"/>
-      <c r="L5" s="38" t="s">
+      <c r="L5" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="38"/>
-      <c r="N5" s="38"/>
-      <c r="O5" s="38"/>
-      <c r="P5" s="37">
+      <c r="M5" s="60"/>
+      <c r="N5" s="60"/>
+      <c r="O5" s="60"/>
+      <c r="P5" s="59">
         <v>42675</v>
       </c>
-      <c r="Q5" s="37"/>
-      <c r="R5" s="37"/>
-      <c r="S5" s="37"/>
-      <c r="T5" s="38" t="s">
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
+      <c r="U5" s="60"/>
+      <c r="V5" s="60"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="AA5" s="38" t="s">
+      <c r="AA5" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="38"/>
-      <c r="AC5" s="38"/>
-      <c r="AD5" s="38"/>
-      <c r="AE5" s="37">
+      <c r="AB5" s="60"/>
+      <c r="AC5" s="60"/>
+      <c r="AD5" s="60"/>
+      <c r="AE5" s="59">
         <v>42713</v>
       </c>
-      <c r="AF5" s="38"/>
-      <c r="AG5" s="38"/>
-      <c r="AH5" s="38"/>
-      <c r="AI5" s="38" t="s">
+      <c r="AF5" s="60"/>
+      <c r="AG5" s="60"/>
+      <c r="AH5" s="60"/>
+      <c r="AI5" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="AJ5" s="38"/>
-      <c r="AK5" s="38"/>
+      <c r="AJ5" s="60"/>
+      <c r="AK5" s="60"/>
       <c r="AW5" s="33"/>
       <c r="AX5" s="33"/>
       <c r="AY5" s="33"/>
@@ -1746,29 +1758,29 @@
     <row r="7" spans="1:57" s="23" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="44"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G7" s="44" t="s">
+      <c r="G7" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="J7" s="44" t="s">
+      <c r="J7" s="40" t="s">
         <v>6</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
@@ -1785,7 +1797,7 @@
       <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AA7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
@@ -1844,7 +1856,7 @@
       <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="44"/>
+      <c r="K8" s="40"/>
       <c r="L8" s="2">
         <v>17</v>
       </c>
@@ -1984,15 +1996,15 @@
     <row r="9" spans="1:57" ht="15.75" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
-      <c r="C9" s="45"/>
+      <c r="C9" s="41"/>
       <c r="D9" s="9"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-      <c r="J9" s="45"/>
-      <c r="K9" s="45"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="2">
         <v>1</v>
       </c>
@@ -2132,14 +2144,14 @@
     </row>
     <row r="10" spans="1:57" ht="19" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="59" t="s">
+      <c r="C10" s="55" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="40" t="s">
+      <c r="E10" s="36" t="s">
         <v>24</v>
       </c>
       <c r="F10" s="11">
@@ -2167,7 +2179,7 @@
       <c r="C11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="6">
@@ -2192,7 +2204,7 @@
       <c r="C12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="35" t="s">
         <v>37</v>
       </c>
       <c r="F12" s="6">
@@ -2215,9 +2227,9 @@
     <row r="13" spans="1:57" ht="19" customHeight="1">
       <c r="A13" s="4"/>
       <c r="C13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F13" s="6">
@@ -2240,7 +2252,7 @@
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F14" s="6">
@@ -2263,7 +2275,7 @@
       <c r="C15" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="39"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="6">
         <v>9</v>
       </c>
@@ -2282,7 +2294,7 @@
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="39"/>
+      <c r="E16" s="35"/>
       <c r="F16" s="6">
         <v>11</v>
       </c>
@@ -2301,7 +2313,7 @@
       <c r="C17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="39"/>
+      <c r="E17" s="35"/>
       <c r="F17" s="6">
         <v>13</v>
       </c>
@@ -2319,10 +2331,10 @@
       <c r="A18" s="8"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="40" t="s">
+      <c r="E18" s="36" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="11">
@@ -2345,12 +2357,12 @@
     </row>
     <row r="19" spans="1:31" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="35" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="6">
@@ -2375,7 +2387,7 @@
       <c r="C20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="35" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="6">
@@ -2400,7 +2412,7 @@
       <c r="C21" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="39" t="s">
+      <c r="E21" s="35" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="6">
@@ -2425,8 +2437,8 @@
       <c r="C22" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="39" t="s">
-        <v>63</v>
+      <c r="E22" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="F22" s="6">
         <v>10</v>
@@ -2446,7 +2458,7 @@
       <c r="C23" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="39" t="s">
+      <c r="E23" s="35" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="6">
@@ -2491,8 +2503,8 @@
       <c r="C24" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="39" t="s">
-        <v>63</v>
+      <c r="E24" s="35" t="s">
+        <v>62</v>
       </c>
       <c r="F24" s="6">
         <v>10</v>
@@ -2509,14 +2521,14 @@
     </row>
     <row r="25" spans="1:31" ht="19" customHeight="1">
       <c r="A25" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B25" s="17"/>
       <c r="C25" s="18" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="17"/>
-      <c r="E25" s="41" t="s">
+      <c r="E25" s="37" t="s">
         <v>31</v>
       </c>
       <c r="F25" s="19">
@@ -2542,7 +2554,7 @@
       <c r="C26" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F26" s="6">
@@ -2567,7 +2579,7 @@
       <c r="C27" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E27" s="39" t="s">
+      <c r="E27" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F27" s="6">
@@ -2612,7 +2624,7 @@
       <c r="C28" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E28" s="39" t="s">
+      <c r="E28" s="35" t="s">
         <v>24</v>
       </c>
       <c r="F28" s="6">
@@ -2659,7 +2671,7 @@
         <v>32</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="36" t="s">
         <v>31</v>
       </c>
       <c r="F29" s="11">
@@ -2682,14 +2694,14 @@
     </row>
     <row r="30" spans="1:31" ht="19" customHeight="1">
       <c r="A30" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B30" s="23"/>
       <c r="C30" s="24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D30" s="23"/>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="38" t="s">
         <v>31</v>
       </c>
       <c r="F30" s="25">
@@ -2714,10 +2726,10 @@
       <c r="A31" s="22"/>
       <c r="B31" s="23"/>
       <c r="C31" s="24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D31" s="23"/>
-      <c r="E31" s="42" t="s">
+      <c r="E31" s="38" t="s">
         <v>31</v>
       </c>
       <c r="F31" s="25">
@@ -2742,10 +2754,10 @@
       <c r="A32" s="22"/>
       <c r="B32" s="23"/>
       <c r="C32" s="24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D32" s="23"/>
-      <c r="E32" s="42" t="s">
+      <c r="E32" s="38" t="s">
         <v>31</v>
       </c>
       <c r="F32" s="25">
@@ -2768,14 +2780,14 @@
     </row>
     <row r="33" spans="1:31" ht="19" customHeight="1">
       <c r="A33" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="17"/>
       <c r="C33" s="18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D33" s="17"/>
-      <c r="E33" s="41" t="s">
+      <c r="E33" s="37" t="s">
         <v>31</v>
       </c>
       <c r="F33" s="19">
@@ -2800,10 +2812,10 @@
       <c r="A34" s="22"/>
       <c r="B34" s="23"/>
       <c r="C34" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D34" s="23"/>
-      <c r="E34" s="42" t="s">
+      <c r="E34" s="38" t="s">
         <v>31</v>
       </c>
       <c r="F34" s="25">
@@ -2828,20 +2840,26 @@
       <c r="A35" s="23"/>
       <c r="B35" s="23"/>
       <c r="C35" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D35" s="23"/>
-      <c r="E35" s="42"/>
+      <c r="E35" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="F35" s="25">
         <v>11</v>
       </c>
       <c r="G35" s="25">
         <v>1</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
+      <c r="H35" s="25">
+        <v>11</v>
+      </c>
+      <c r="I35" s="25">
+        <v>1</v>
+      </c>
       <c r="J35" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="27"/>
       <c r="AA35" s="29"/>
@@ -2850,12 +2868,12 @@
       <c r="A36" s="22"/>
       <c r="B36" s="23"/>
       <c r="C36" s="24" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="23"/>
-      <c r="E36" s="42"/>
+      <c r="E36" s="38"/>
       <c r="F36" s="25">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G36" s="25">
         <v>1</v>
@@ -2868,165 +2886,157 @@
       <c r="K36" s="27"/>
       <c r="AA36" s="29"/>
     </row>
-    <row r="37" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A37" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="41" t="s">
+    <row r="37" spans="1:31" ht="19" customHeight="1">
+      <c r="A37" s="22"/>
+      <c r="B37" s="23"/>
+      <c r="C37" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="23"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="25">
+        <v>12</v>
+      </c>
+      <c r="G37" s="25">
+        <v>1</v>
+      </c>
+      <c r="H37" s="25"/>
+      <c r="I37" s="25"/>
+      <c r="J37" s="26">
+        <v>0</v>
+      </c>
+      <c r="K37" s="27"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
+      <c r="O37" s="34"/>
+      <c r="P37" s="34"/>
+      <c r="Q37" s="34"/>
+      <c r="R37" s="34"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="34"/>
+      <c r="U37" s="34"/>
+      <c r="V37" s="34"/>
+      <c r="W37" s="34"/>
+      <c r="X37" s="34"/>
+      <c r="Y37" s="34"/>
+      <c r="Z37" s="34"/>
+      <c r="AA37" s="29"/>
+      <c r="AB37" s="34"/>
+      <c r="AC37" s="34"/>
+      <c r="AD37" s="34"/>
+      <c r="AE37" s="34"/>
+    </row>
+    <row r="38" spans="1:31" ht="19" customHeight="1">
+      <c r="A38" s="22"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="23"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="25">
+        <v>14</v>
+      </c>
+      <c r="G38" s="25">
+        <v>1</v>
+      </c>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="26">
+        <v>0</v>
+      </c>
+      <c r="K38" s="27"/>
+      <c r="L38" s="34"/>
+      <c r="M38" s="34"/>
+      <c r="N38" s="34"/>
+      <c r="O38" s="34"/>
+      <c r="P38" s="34"/>
+      <c r="Q38" s="34"/>
+      <c r="R38" s="34"/>
+      <c r="S38" s="34"/>
+      <c r="T38" s="34"/>
+      <c r="U38" s="34"/>
+      <c r="V38" s="34"/>
+      <c r="W38" s="34"/>
+      <c r="X38" s="34"/>
+      <c r="Y38" s="34"/>
+      <c r="Z38" s="34"/>
+      <c r="AA38" s="29"/>
+      <c r="AB38" s="34"/>
+      <c r="AC38" s="34"/>
+      <c r="AD38" s="34"/>
+      <c r="AE38" s="34"/>
+    </row>
+    <row r="39" spans="1:31" ht="19" customHeight="1">
+      <c r="A39" s="22"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" s="23"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="25">
+        <v>14</v>
+      </c>
+      <c r="G39" s="25">
+        <v>1</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="26">
+        <v>0</v>
+      </c>
+      <c r="K39" s="27"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="34"/>
+      <c r="N39" s="34"/>
+      <c r="O39" s="34"/>
+      <c r="P39" s="34"/>
+      <c r="Q39" s="34"/>
+      <c r="R39" s="34"/>
+      <c r="S39" s="34"/>
+      <c r="T39" s="34"/>
+      <c r="U39" s="34"/>
+      <c r="V39" s="34"/>
+      <c r="W39" s="34"/>
+      <c r="X39" s="34"/>
+      <c r="Y39" s="34"/>
+      <c r="Z39" s="34"/>
+      <c r="AA39" s="29"/>
+      <c r="AB39" s="34"/>
+      <c r="AC39" s="34"/>
+      <c r="AD39" s="34"/>
+      <c r="AE39" s="34"/>
+    </row>
+    <row r="40" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
+      <c r="A40" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="17"/>
+      <c r="E40" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="F37" s="19">
+      <c r="F40" s="19">
         <v>6</v>
       </c>
-      <c r="G37" s="19">
-        <v>1</v>
-      </c>
-      <c r="H37" s="19">
+      <c r="G40" s="19">
+        <v>1</v>
+      </c>
+      <c r="H40" s="19">
         <v>6</v>
       </c>
-      <c r="I37" s="19">
-        <v>1</v>
-      </c>
-      <c r="J37" s="20">
-        <v>1</v>
-      </c>
-      <c r="K37" s="21"/>
-      <c r="L37" s="27"/>
-      <c r="M37" s="27"/>
-      <c r="N37" s="27"/>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="27"/>
-      <c r="S37" s="27"/>
-      <c r="T37" s="27"/>
-      <c r="U37" s="27"/>
-      <c r="V37" s="27"/>
-      <c r="W37" s="27"/>
-      <c r="X37" s="27"/>
-      <c r="Y37" s="27"/>
-      <c r="Z37" s="27"/>
-      <c r="AA37" s="31"/>
-      <c r="AB37" s="27"/>
-      <c r="AC37" s="27"/>
-      <c r="AD37" s="27"/>
-      <c r="AE37" s="27"/>
-    </row>
-    <row r="38" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A38" s="22"/>
-      <c r="C38" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F38" s="25">
-        <v>6</v>
-      </c>
-      <c r="G38" s="25">
-        <v>1</v>
-      </c>
-      <c r="H38" s="25">
-        <v>6</v>
-      </c>
-      <c r="I38" s="25">
-        <v>1</v>
-      </c>
-      <c r="J38" s="26">
-        <v>1</v>
-      </c>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
-      <c r="Q38" s="27"/>
-      <c r="R38" s="27"/>
-      <c r="S38" s="27"/>
-      <c r="T38" s="27"/>
-      <c r="U38" s="27"/>
-      <c r="V38" s="27"/>
-      <c r="W38" s="27"/>
-      <c r="X38" s="27"/>
-      <c r="Y38" s="27"/>
-      <c r="Z38" s="27"/>
-      <c r="AA38" s="31"/>
-      <c r="AB38" s="27"/>
-      <c r="AC38" s="27"/>
-      <c r="AD38" s="27"/>
-      <c r="AE38" s="27"/>
-    </row>
-    <row r="39" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A39" s="22"/>
-      <c r="C39" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="25">
-        <v>10</v>
-      </c>
-      <c r="G39" s="25">
-        <v>1</v>
-      </c>
-      <c r="H39" s="25">
-        <v>10</v>
-      </c>
-      <c r="I39" s="25">
-        <v>1</v>
-      </c>
-      <c r="J39" s="26">
-        <v>1</v>
-      </c>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
-      <c r="M39" s="27"/>
-      <c r="N39" s="27"/>
-      <c r="O39" s="27"/>
-      <c r="P39" s="27"/>
-      <c r="Q39" s="27"/>
-      <c r="R39" s="27"/>
-      <c r="S39" s="27"/>
-      <c r="T39" s="27"/>
-      <c r="U39" s="27"/>
-      <c r="V39" s="27"/>
-      <c r="W39" s="27"/>
-      <c r="X39" s="27"/>
-      <c r="Y39" s="27"/>
-      <c r="Z39" s="27"/>
-      <c r="AA39" s="31"/>
-      <c r="AB39" s="27"/>
-      <c r="AC39" s="27"/>
-      <c r="AD39" s="27"/>
-      <c r="AE39" s="27"/>
-    </row>
-    <row r="40" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A40" s="22"/>
-      <c r="C40" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>63</v>
-      </c>
-      <c r="F40" s="25">
-        <v>11</v>
-      </c>
-      <c r="G40" s="25">
-        <v>1</v>
-      </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="26">
-        <v>0</v>
-      </c>
-      <c r="K40" s="27"/>
+      <c r="I40" s="19">
+        <v>1</v>
+      </c>
+      <c r="J40" s="20">
+        <v>1</v>
+      </c>
+      <c r="K40" s="21"/>
       <c r="L40" s="27"/>
       <c r="M40" s="27"/>
       <c r="N40" s="27"/>
@@ -3051,19 +3061,25 @@
     <row r="41" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A41" s="22"/>
       <c r="C41" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="E41" s="42"/>
+        <v>52</v>
+      </c>
+      <c r="E41" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="F41" s="25">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="G41" s="25">
-        <v>2</v>
-      </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="H41" s="25">
+        <v>6</v>
+      </c>
+      <c r="I41" s="25">
+        <v>1</v>
+      </c>
       <c r="J41" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="27"/>
       <c r="L41" s="27"/>
@@ -3090,21 +3106,25 @@
     <row r="42" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A42" s="22"/>
       <c r="C42" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+      <c r="E42" s="38" t="s">
+        <v>31</v>
       </c>
       <c r="F42" s="25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G42" s="25">
         <v>1</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
+      <c r="H42" s="25">
+        <v>10</v>
+      </c>
+      <c r="I42" s="25">
+        <v>1</v>
+      </c>
       <c r="J42" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="27"/>
       <c r="L42" s="27"/>
@@ -3131,9 +3151,11 @@
     <row r="43" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A43" s="22"/>
       <c r="C43" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="E43" s="42"/>
+        <v>53</v>
+      </c>
+      <c r="E43" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="F43" s="25">
         <v>11</v>
       </c>
@@ -3168,27 +3190,23 @@
       <c r="AE43" s="27"/>
     </row>
     <row r="44" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A44" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="D44" s="17"/>
-      <c r="E44" s="41"/>
-      <c r="F44" s="19">
-        <v>11</v>
-      </c>
-      <c r="G44" s="19">
-        <v>1</v>
-      </c>
-      <c r="H44" s="19"/>
-      <c r="I44" s="19"/>
-      <c r="J44" s="20">
+      <c r="A44" s="22"/>
+      <c r="C44" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E44" s="38"/>
+      <c r="F44" s="25">
+        <v>12</v>
+      </c>
+      <c r="G44" s="25">
+        <v>2</v>
+      </c>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="26">
         <v>0</v>
       </c>
-      <c r="K44" s="21"/>
+      <c r="K44" s="27"/>
       <c r="L44" s="27"/>
       <c r="M44" s="27"/>
       <c r="N44" s="27"/>
@@ -3213,14 +3231,16 @@
     <row r="45" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A45" s="22"/>
       <c r="C45" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" s="42"/>
+        <v>54</v>
+      </c>
+      <c r="E45" s="38" t="s">
+        <v>62</v>
+      </c>
       <c r="F45" s="25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G45" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" s="25"/>
       <c r="I45" s="25"/>
@@ -3252,9 +3272,9 @@
     <row r="46" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A46" s="22"/>
       <c r="C46" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E46" s="42"/>
+        <v>68</v>
+      </c>
+      <c r="E46" s="38"/>
       <c r="F46" s="25">
         <v>11</v>
       </c>
@@ -3289,23 +3309,29 @@
       <c r="AE46" s="27"/>
     </row>
     <row r="47" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A47" s="22"/>
-      <c r="C47" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" s="42"/>
-      <c r="F47" s="25">
-        <v>12</v>
-      </c>
-      <c r="G47" s="25">
-        <v>1</v>
-      </c>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="26">
-        <v>0</v>
-      </c>
-      <c r="K47" s="27"/>
+      <c r="A47" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D47" s="17"/>
+      <c r="E47" s="37"/>
+      <c r="F47" s="19">
+        <v>11</v>
+      </c>
+      <c r="G47" s="19">
+        <v>2</v>
+      </c>
+      <c r="H47" s="19">
+        <v>11</v>
+      </c>
+      <c r="I47" s="19"/>
+      <c r="J47" s="20">
+        <v>0.25</v>
+      </c>
+      <c r="K47" s="21"/>
       <c r="L47" s="27"/>
       <c r="M47" s="27"/>
       <c r="N47" s="27"/>
@@ -3328,27 +3354,23 @@
       <c r="AE47" s="27"/>
     </row>
     <row r="48" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A48" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D48" s="17"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="19">
-        <v>1</v>
-      </c>
-      <c r="G48" s="19">
-        <v>1</v>
-      </c>
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
-      <c r="J48" s="20">
+      <c r="A48" s="22"/>
+      <c r="C48" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="38"/>
+      <c r="F48" s="25">
+        <v>13</v>
+      </c>
+      <c r="G48" s="25">
+        <v>2</v>
+      </c>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="26">
         <v>0</v>
       </c>
-      <c r="K48" s="21"/>
+      <c r="K48" s="27"/>
       <c r="L48" s="27"/>
       <c r="M48" s="27"/>
       <c r="N48" s="27"/>
@@ -3373,11 +3395,11 @@
     <row r="49" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A49" s="22"/>
       <c r="C49" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="E49" s="42"/>
+        <v>70</v>
+      </c>
+      <c r="E49" s="38"/>
       <c r="F49" s="25">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="G49" s="25">
         <v>2</v>
@@ -3412,11 +3434,11 @@
     <row r="50" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A50" s="22"/>
       <c r="C50" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E50" s="42"/>
+        <v>72</v>
+      </c>
+      <c r="E50" s="38"/>
       <c r="F50" s="25">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G50" s="25">
         <v>1</v>
@@ -3449,23 +3471,27 @@
       <c r="AE50" s="27"/>
     </row>
     <row r="51" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A51" s="22"/>
-      <c r="C51" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" s="42"/>
-      <c r="F51" s="25">
-        <v>1</v>
-      </c>
-      <c r="G51" s="25">
-        <v>1</v>
-      </c>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="26">
+      <c r="A51" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="17"/>
+      <c r="C51" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51" s="17"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="19">
+        <v>1</v>
+      </c>
+      <c r="G51" s="19">
+        <v>1</v>
+      </c>
+      <c r="H51" s="19"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="20">
         <v>0</v>
       </c>
-      <c r="K51" s="27"/>
+      <c r="K51" s="21"/>
       <c r="L51" s="27"/>
       <c r="M51" s="27"/>
       <c r="N51" s="27"/>
@@ -3490,9 +3516,9 @@
     <row r="52" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A52" s="22"/>
       <c r="C52" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E52" s="42"/>
+        <v>78</v>
+      </c>
+      <c r="E52" s="38"/>
       <c r="F52" s="25">
         <v>1</v>
       </c>
@@ -3529,14 +3555,14 @@
     <row r="53" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A53" s="22"/>
       <c r="C53" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" s="42"/>
+        <v>79</v>
+      </c>
+      <c r="E53" s="38"/>
       <c r="F53" s="25">
         <v>1</v>
       </c>
       <c r="G53" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H53" s="25"/>
       <c r="I53" s="25"/>
@@ -3568,9 +3594,9 @@
     <row r="54" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A54" s="22"/>
       <c r="C54" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E54" s="42"/>
+        <v>56</v>
+      </c>
+      <c r="E54" s="38"/>
       <c r="F54" s="25">
         <v>1</v>
       </c>
@@ -3607,14 +3633,14 @@
     <row r="55" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A55" s="22"/>
       <c r="C55" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E55" s="42"/>
+        <v>61</v>
+      </c>
+      <c r="E55" s="38"/>
       <c r="F55" s="25">
         <v>1</v>
       </c>
       <c r="G55" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
@@ -3646,14 +3672,14 @@
     <row r="56" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A56" s="22"/>
       <c r="C56" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E56" s="42"/>
+        <v>80</v>
+      </c>
+      <c r="E56" s="38"/>
       <c r="F56" s="25">
         <v>1</v>
       </c>
       <c r="G56" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H56" s="25"/>
       <c r="I56" s="25"/>
@@ -3685,14 +3711,14 @@
     <row r="57" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A57" s="22"/>
       <c r="C57" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E57" s="42"/>
+        <v>57</v>
+      </c>
+      <c r="E57" s="38"/>
       <c r="F57" s="25">
         <v>1</v>
       </c>
       <c r="G57" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
@@ -3724,14 +3750,14 @@
     <row r="58" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A58" s="22"/>
       <c r="C58" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E58" s="42"/>
+        <v>81</v>
+      </c>
+      <c r="E58" s="38"/>
       <c r="F58" s="25">
         <v>1</v>
       </c>
       <c r="G58" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
@@ -3763,14 +3789,14 @@
     <row r="59" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A59" s="22"/>
       <c r="C59" s="24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E59" s="42"/>
+        <v>82</v>
+      </c>
+      <c r="E59" s="38"/>
       <c r="F59" s="25">
         <v>1</v>
       </c>
       <c r="G59" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
@@ -3800,25 +3826,23 @@
       <c r="AE59" s="27"/>
     </row>
     <row r="60" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A60" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="B60" s="17"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="19">
-        <v>1</v>
-      </c>
-      <c r="G60" s="19">
-        <v>1</v>
-      </c>
-      <c r="H60" s="19"/>
-      <c r="I60" s="19"/>
-      <c r="J60" s="20">
+      <c r="A60" s="22"/>
+      <c r="C60" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" s="38"/>
+      <c r="F60" s="25">
+        <v>1</v>
+      </c>
+      <c r="G60" s="25">
+        <v>3</v>
+      </c>
+      <c r="H60" s="25"/>
+      <c r="I60" s="25"/>
+      <c r="J60" s="26">
         <v>0</v>
       </c>
-      <c r="K60" s="21"/>
+      <c r="K60" s="27"/>
       <c r="L60" s="27"/>
       <c r="M60" s="27"/>
       <c r="N60" s="27"/>
@@ -3842,13 +3866,15 @@
     </row>
     <row r="61" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A61" s="22"/>
-      <c r="C61" s="24"/>
-      <c r="E61" s="42"/>
+      <c r="C61" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E61" s="38"/>
       <c r="F61" s="25">
         <v>1</v>
       </c>
       <c r="G61" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H61" s="25"/>
       <c r="I61" s="25"/>
@@ -3879,13 +3905,15 @@
     </row>
     <row r="62" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A62" s="22"/>
-      <c r="C62" s="24"/>
-      <c r="E62" s="42"/>
+      <c r="C62" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E62" s="38"/>
       <c r="F62" s="25">
         <v>1</v>
       </c>
       <c r="G62" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="25"/>
@@ -3915,21 +3943,25 @@
       <c r="AE62" s="27"/>
     </row>
     <row r="63" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A63" s="22"/>
-      <c r="C63" s="24"/>
-      <c r="E63" s="42"/>
-      <c r="F63" s="25">
-        <v>1</v>
-      </c>
-      <c r="G63" s="25">
-        <v>1</v>
-      </c>
-      <c r="H63" s="25"/>
-      <c r="I63" s="25"/>
-      <c r="J63" s="26">
+      <c r="A63" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63" s="17"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="19">
+        <v>1</v>
+      </c>
+      <c r="G63" s="19">
+        <v>1</v>
+      </c>
+      <c r="H63" s="19"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="20">
         <v>0</v>
       </c>
-      <c r="K63" s="27"/>
+      <c r="K63" s="21"/>
       <c r="L63" s="27"/>
       <c r="M63" s="27"/>
       <c r="N63" s="27"/>
@@ -3954,7 +3986,7 @@
     <row r="64" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A64" s="22"/>
       <c r="C64" s="24"/>
-      <c r="E64" s="42"/>
+      <c r="E64" s="38"/>
       <c r="F64" s="25">
         <v>1</v>
       </c>
@@ -3991,7 +4023,7 @@
     <row r="65" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A65" s="22"/>
       <c r="C65" s="24"/>
-      <c r="E65" s="42"/>
+      <c r="E65" s="38"/>
       <c r="F65" s="25">
         <v>1</v>
       </c>
@@ -4028,7 +4060,7 @@
     <row r="66" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A66" s="22"/>
       <c r="C66" s="24"/>
-      <c r="E66" s="42"/>
+      <c r="E66" s="38"/>
       <c r="F66" s="25">
         <v>1</v>
       </c>
@@ -4065,7 +4097,7 @@
     <row r="67" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A67" s="22"/>
       <c r="C67" s="24"/>
-      <c r="E67" s="42"/>
+      <c r="E67" s="38"/>
       <c r="F67" s="25">
         <v>1</v>
       </c>
@@ -4102,7 +4134,7 @@
     <row r="68" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A68" s="22"/>
       <c r="C68" s="24"/>
-      <c r="E68" s="42"/>
+      <c r="E68" s="38"/>
       <c r="F68" s="25">
         <v>1</v>
       </c>
@@ -4139,7 +4171,7 @@
     <row r="69" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A69" s="22"/>
       <c r="C69" s="24"/>
-      <c r="E69" s="42"/>
+      <c r="E69" s="38"/>
       <c r="F69" s="25">
         <v>1</v>
       </c>
@@ -4176,7 +4208,7 @@
     <row r="70" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A70" s="22"/>
       <c r="C70" s="24"/>
-      <c r="E70" s="42"/>
+      <c r="E70" s="38"/>
       <c r="F70" s="25">
         <v>1</v>
       </c>
@@ -4210,6 +4242,117 @@
       <c r="AD70" s="27"/>
       <c r="AE70" s="27"/>
     </row>
+    <row r="71" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
+      <c r="A71" s="22"/>
+      <c r="C71" s="24"/>
+      <c r="E71" s="38"/>
+      <c r="F71" s="25">
+        <v>1</v>
+      </c>
+      <c r="G71" s="25">
+        <v>1</v>
+      </c>
+      <c r="H71" s="25"/>
+      <c r="I71" s="25"/>
+      <c r="J71" s="26">
+        <v>0</v>
+      </c>
+      <c r="K71" s="27"/>
+      <c r="L71" s="27"/>
+      <c r="M71" s="27"/>
+      <c r="N71" s="27"/>
+      <c r="O71" s="27"/>
+      <c r="P71" s="27"/>
+      <c r="Q71" s="27"/>
+      <c r="R71" s="27"/>
+      <c r="S71" s="27"/>
+      <c r="T71" s="27"/>
+      <c r="U71" s="27"/>
+      <c r="V71" s="27"/>
+      <c r="W71" s="27"/>
+      <c r="X71" s="27"/>
+      <c r="Y71" s="27"/>
+      <c r="Z71" s="27"/>
+      <c r="AA71" s="31"/>
+      <c r="AB71" s="27"/>
+      <c r="AC71" s="27"/>
+      <c r="AD71" s="27"/>
+      <c r="AE71" s="27"/>
+    </row>
+    <row r="72" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
+      <c r="A72" s="22"/>
+      <c r="C72" s="24"/>
+      <c r="E72" s="38"/>
+      <c r="F72" s="25">
+        <v>1</v>
+      </c>
+      <c r="G72" s="25">
+        <v>1</v>
+      </c>
+      <c r="H72" s="25"/>
+      <c r="I72" s="25"/>
+      <c r="J72" s="26">
+        <v>0</v>
+      </c>
+      <c r="K72" s="27"/>
+      <c r="L72" s="27"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="27"/>
+      <c r="Q72" s="27"/>
+      <c r="R72" s="27"/>
+      <c r="S72" s="27"/>
+      <c r="T72" s="27"/>
+      <c r="U72" s="27"/>
+      <c r="V72" s="27"/>
+      <c r="W72" s="27"/>
+      <c r="X72" s="27"/>
+      <c r="Y72" s="27"/>
+      <c r="Z72" s="27"/>
+      <c r="AA72" s="31"/>
+      <c r="AB72" s="27"/>
+      <c r="AC72" s="27"/>
+      <c r="AD72" s="27"/>
+      <c r="AE72" s="27"/>
+    </row>
+    <row r="73" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
+      <c r="A73" s="22"/>
+      <c r="C73" s="24"/>
+      <c r="E73" s="38"/>
+      <c r="F73" s="25">
+        <v>1</v>
+      </c>
+      <c r="G73" s="25">
+        <v>1</v>
+      </c>
+      <c r="H73" s="25"/>
+      <c r="I73" s="25"/>
+      <c r="J73" s="26">
+        <v>0</v>
+      </c>
+      <c r="K73" s="27"/>
+      <c r="L73" s="27"/>
+      <c r="M73" s="27"/>
+      <c r="N73" s="27"/>
+      <c r="O73" s="27"/>
+      <c r="P73" s="27"/>
+      <c r="Q73" s="27"/>
+      <c r="R73" s="27"/>
+      <c r="S73" s="27"/>
+      <c r="T73" s="27"/>
+      <c r="U73" s="27"/>
+      <c r="V73" s="27"/>
+      <c r="W73" s="27"/>
+      <c r="X73" s="27"/>
+      <c r="Y73" s="27"/>
+      <c r="Z73" s="27"/>
+      <c r="AA73" s="31"/>
+      <c r="AB73" s="27"/>
+      <c r="AC73" s="27"/>
+      <c r="AD73" s="27"/>
+      <c r="AE73" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="AR4:AU4"/>
@@ -4227,7 +4370,7 @@
     <mergeCell ref="AI5:AK5"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="L10:BD70">
+  <conditionalFormatting sqref="L10:BD73">
     <cfRule type="expression" dxfId="9" priority="50">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
update review data and create overall ratings section of the page
</commit_message>
<xml_diff>
--- a/documentation/ESAP_Gantt_Chart.xlsx
+++ b/documentation/ESAP_Gantt_Chart.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="93">
   <si>
     <t>Plan</t>
   </si>
@@ -366,13 +366,16 @@
     <t>Update collection schemas</t>
   </si>
   <si>
-    <t>Make buildings collection generic for all types</t>
-  </si>
-  <si>
     <t>Come up with schema for ratings (i.e. what to rate)</t>
   </si>
   <si>
     <t>Design</t>
+  </si>
+  <si>
+    <t>Add feature for user log in /sign up</t>
+  </si>
+  <si>
+    <t>Get data for a building from the backend</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -970,9 +973,6 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="7" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1006,6 +1006,9 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1019,6 +1022,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1266,7 +1272,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="12"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="15"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1545,27 +1551,27 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BE73"/>
+  <dimension ref="A2:BE74"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48" style="52" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.6640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="8.1640625" style="39" customWidth="1"/>
     <col min="6" max="6" width="7.1640625" style="33" customWidth="1"/>
     <col min="7" max="7" width="9.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" style="33" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="33" customWidth="1"/>
-    <col min="10" max="10" width="7.1640625" style="54" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="53" customWidth="1"/>
     <col min="11" max="11" width="2.83203125" style="33" customWidth="1"/>
     <col min="12" max="16" width="3.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="18" max="27" width="3.1640625" style="33" bestFit="1" customWidth="1"/>
     <col min="28" max="31" width="2.83203125" style="33" bestFit="1" customWidth="1"/>
     <col min="32" max="35" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
@@ -1599,33 +1605,33 @@
       <c r="N2" s="43"/>
       <c r="O2" s="43"/>
       <c r="P2" s="43"/>
-      <c r="Q2" s="44">
-        <f ca="1">DAYS360(P4,today+1)</f>
-        <v>12</v>
+      <c r="Q2" s="61">
+        <f ca="1">DAYS360(P4 - 1,today)</f>
+        <v>15</v>
       </c>
       <c r="R2" s="43"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="46" t="s">
+      <c r="T2" s="44"/>
+      <c r="U2" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="W2" s="47"/>
-      <c r="X2" s="46" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="49" t="s">
+      <c r="W2" s="46"/>
+      <c r="X2" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="47"/>
+      <c r="AB2" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="49" t="s">
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="48" t="s">
         <v>9</v>
       </c>
       <c r="AJ2" s="33"/>
       <c r="AK2" s="33"/>
       <c r="AL2" s="33"/>
       <c r="AM2" s="33"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="49" t="s">
+      <c r="AN2" s="50"/>
+      <c r="AO2" s="48" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1678,12 +1684,12 @@
       <c r="AI4" s="33"/>
       <c r="AJ4" s="33"/>
       <c r="AK4" s="33"/>
-      <c r="AN4" s="52" t="s">
+      <c r="AN4" s="51" t="s">
         <v>48</v>
       </c>
       <c r="AR4" s="56">
         <f ca="1">TODAY()</f>
-        <v>42671</v>
+        <v>42675</v>
       </c>
       <c r="AS4" s="56"/>
       <c r="AT4" s="56"/>
@@ -2147,7 +2153,7 @@
         <v>55</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="55" t="s">
+      <c r="C10" s="54" t="s">
         <v>29</v>
       </c>
       <c r="D10" s="9"/>
@@ -2357,7 +2363,7 @@
     </row>
     <row r="19" spans="1:31" ht="19" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>33</v>
@@ -2898,7 +2904,7 @@
       <c r="A37" s="22"/>
       <c r="B37" s="23"/>
       <c r="C37" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" s="23"/>
       <c r="E37" s="38" t="s">
@@ -2990,42 +2996,40 @@
       <c r="A39" s="22"/>
       <c r="B39" s="23"/>
       <c r="C39" s="24" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D39" s="23"/>
       <c r="E39" s="38"/>
       <c r="F39" s="25">
-        <v>14</v>
-      </c>
-      <c r="G39" s="25">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="G39" s="25"/>
       <c r="H39" s="25"/>
       <c r="I39" s="25"/>
       <c r="J39" s="26">
         <v>0</v>
       </c>
       <c r="K39" s="27"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="34"/>
-      <c r="Q39" s="34"/>
-      <c r="R39" s="34"/>
-      <c r="S39" s="34"/>
-      <c r="T39" s="34"/>
-      <c r="U39" s="34"/>
-      <c r="V39" s="34"/>
-      <c r="W39" s="34"/>
-      <c r="X39" s="34"/>
-      <c r="Y39" s="34"/>
-      <c r="Z39" s="34"/>
+      <c r="L39" s="55"/>
+      <c r="M39" s="55"/>
+      <c r="N39" s="55"/>
+      <c r="O39" s="55"/>
+      <c r="P39" s="55"/>
+      <c r="Q39" s="55"/>
+      <c r="R39" s="55"/>
+      <c r="S39" s="55"/>
+      <c r="T39" s="55"/>
+      <c r="U39" s="55"/>
+      <c r="V39" s="55"/>
+      <c r="W39" s="55"/>
+      <c r="X39" s="55"/>
+      <c r="Y39" s="55"/>
+      <c r="Z39" s="55"/>
       <c r="AA39" s="29"/>
-      <c r="AB39" s="34"/>
-      <c r="AC39" s="34"/>
-      <c r="AD39" s="34"/>
-      <c r="AE39" s="34"/>
+      <c r="AB39" s="55"/>
+      <c r="AC39" s="55"/>
+      <c r="AD39" s="55"/>
+      <c r="AE39" s="55"/>
     </row>
     <row r="40" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A40" s="16" t="s">
@@ -3335,7 +3339,9 @@
         <v>69</v>
       </c>
       <c r="D47" s="17"/>
-      <c r="E47" s="37"/>
+      <c r="E47" s="37" t="s">
+        <v>37</v>
+      </c>
       <c r="F47" s="19">
         <v>11</v>
       </c>
@@ -3376,7 +3382,9 @@
       <c r="C48" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="E48" s="38"/>
+      <c r="E48" s="38" t="s">
+        <v>37</v>
+      </c>
       <c r="F48" s="25">
         <v>13</v>
       </c>
@@ -3415,7 +3423,9 @@
       <c r="C49" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="E49" s="38"/>
+      <c r="E49" s="38" t="s">
+        <v>37</v>
+      </c>
       <c r="F49" s="25">
         <v>11</v>
       </c>
@@ -3454,7 +3464,9 @@
       <c r="C50" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="E50" s="38"/>
+      <c r="E50" s="38" t="s">
+        <v>37</v>
+      </c>
       <c r="F50" s="25">
         <v>13</v>
       </c>
@@ -3497,17 +3509,23 @@
         <v>75</v>
       </c>
       <c r="D51" s="17"/>
-      <c r="E51" s="37"/>
+      <c r="E51" s="37" t="s">
+        <v>31</v>
+      </c>
       <c r="F51" s="19">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G51" s="19">
         <v>1</v>
       </c>
-      <c r="H51" s="19"/>
-      <c r="I51" s="19"/>
+      <c r="H51" s="19">
+        <v>15</v>
+      </c>
+      <c r="I51" s="19">
+        <v>1</v>
+      </c>
       <c r="J51" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" s="21"/>
       <c r="L51" s="27"/>
@@ -3536,17 +3554,23 @@
       <c r="C52" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E52" s="38"/>
+      <c r="E52" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="F52" s="25">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G52" s="25">
-        <v>2</v>
-      </c>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
+        <v>1</v>
+      </c>
+      <c r="H52" s="25">
+        <v>15</v>
+      </c>
+      <c r="I52" s="25">
+        <v>1</v>
+      </c>
       <c r="J52" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="27"/>
       <c r="L52" s="27"/>
@@ -3575,17 +3599,23 @@
       <c r="C53" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="E53" s="38"/>
+      <c r="E53" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="F53" s="25">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G53" s="25">
         <v>1</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
+      <c r="H53" s="25">
+        <v>15</v>
+      </c>
+      <c r="I53" s="25">
+        <v>1</v>
+      </c>
       <c r="J53" s="26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="27"/>
       <c r="L53" s="27"/>
@@ -3612,19 +3642,25 @@
     <row r="54" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A54" s="22"/>
       <c r="C54" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="38"/>
+        <v>92</v>
+      </c>
+      <c r="E54" s="38" t="s">
+        <v>31</v>
+      </c>
       <c r="F54" s="25">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G54" s="25">
-        <v>1</v>
-      </c>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
+        <v>2</v>
+      </c>
+      <c r="H54" s="25">
+        <v>15</v>
+      </c>
+      <c r="I54" s="25">
+        <v>2</v>
+      </c>
       <c r="J54" s="26">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="K54" s="27"/>
       <c r="L54" s="27"/>
@@ -3651,14 +3687,14 @@
     <row r="55" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A55" s="22"/>
       <c r="C55" s="24" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E55" s="38"/>
       <c r="F55" s="25">
         <v>1</v>
       </c>
       <c r="G55" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H55" s="25"/>
       <c r="I55" s="25"/>
@@ -3690,14 +3726,14 @@
     <row r="56" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A56" s="22"/>
       <c r="C56" s="24" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E56" s="38"/>
       <c r="F56" s="25">
         <v>1</v>
       </c>
       <c r="G56" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H56" s="25"/>
       <c r="I56" s="25"/>
@@ -3729,14 +3765,14 @@
     <row r="57" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A57" s="22"/>
       <c r="C57" s="24" t="s">
-        <v>57</v>
+        <v>80</v>
       </c>
       <c r="E57" s="38"/>
       <c r="F57" s="25">
         <v>1</v>
       </c>
       <c r="G57" s="25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H57" s="25"/>
       <c r="I57" s="25"/>
@@ -3768,14 +3804,14 @@
     <row r="58" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A58" s="22"/>
       <c r="C58" s="24" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="E58" s="38"/>
       <c r="F58" s="25">
         <v>1</v>
       </c>
       <c r="G58" s="25">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H58" s="25"/>
       <c r="I58" s="25"/>
@@ -3807,14 +3843,14 @@
     <row r="59" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A59" s="22"/>
       <c r="C59" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E59" s="38"/>
       <c r="F59" s="25">
         <v>1</v>
       </c>
       <c r="G59" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H59" s="25"/>
       <c r="I59" s="25"/>
@@ -3846,14 +3882,14 @@
     <row r="60" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A60" s="22"/>
       <c r="C60" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E60" s="38"/>
       <c r="F60" s="25">
         <v>1</v>
       </c>
       <c r="G60" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H60" s="25"/>
       <c r="I60" s="25"/>
@@ -3885,14 +3921,14 @@
     <row r="61" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A61" s="22"/>
       <c r="C61" s="24" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="E61" s="38"/>
       <c r="F61" s="25">
         <v>1</v>
       </c>
       <c r="G61" s="25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H61" s="25"/>
       <c r="I61" s="25"/>
@@ -3924,14 +3960,14 @@
     <row r="62" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
       <c r="A62" s="22"/>
       <c r="C62" s="24" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E62" s="38"/>
       <c r="F62" s="25">
         <v>1</v>
       </c>
       <c r="G62" s="25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H62" s="25"/>
       <c r="I62" s="25"/>
@@ -3961,25 +3997,23 @@
       <c r="AE62" s="27"/>
     </row>
     <row r="63" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A63" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="17"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="19">
-        <v>1</v>
-      </c>
-      <c r="G63" s="19">
-        <v>1</v>
-      </c>
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
-      <c r="J63" s="20">
+      <c r="A63" s="22"/>
+      <c r="C63" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" s="38"/>
+      <c r="F63" s="25">
+        <v>1</v>
+      </c>
+      <c r="G63" s="25">
+        <v>3</v>
+      </c>
+      <c r="H63" s="25"/>
+      <c r="I63" s="25"/>
+      <c r="J63" s="26">
         <v>0</v>
       </c>
-      <c r="K63" s="21"/>
+      <c r="K63" s="27"/>
       <c r="L63" s="27"/>
       <c r="M63" s="27"/>
       <c r="N63" s="27"/>
@@ -4002,21 +4036,25 @@
       <c r="AE63" s="27"/>
     </row>
     <row r="64" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
-      <c r="A64" s="22"/>
-      <c r="C64" s="24"/>
-      <c r="E64" s="38"/>
-      <c r="F64" s="25">
-        <v>1</v>
-      </c>
-      <c r="G64" s="25">
-        <v>1</v>
-      </c>
-      <c r="H64" s="25"/>
-      <c r="I64" s="25"/>
-      <c r="J64" s="26">
+      <c r="A64" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B64" s="17"/>
+      <c r="C64" s="18"/>
+      <c r="D64" s="17"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="19">
+        <v>1</v>
+      </c>
+      <c r="G64" s="19">
+        <v>1</v>
+      </c>
+      <c r="H64" s="19"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="20">
         <v>0</v>
       </c>
-      <c r="K64" s="27"/>
+      <c r="K64" s="21"/>
       <c r="L64" s="27"/>
       <c r="M64" s="27"/>
       <c r="N64" s="27"/>
@@ -4371,6 +4409,43 @@
       <c r="AD73" s="27"/>
       <c r="AE73" s="27"/>
     </row>
+    <row r="74" spans="1:31" s="23" customFormat="1" ht="19" customHeight="1">
+      <c r="A74" s="22"/>
+      <c r="C74" s="24"/>
+      <c r="E74" s="38"/>
+      <c r="F74" s="25">
+        <v>1</v>
+      </c>
+      <c r="G74" s="25">
+        <v>1</v>
+      </c>
+      <c r="H74" s="25"/>
+      <c r="I74" s="25"/>
+      <c r="J74" s="26">
+        <v>0</v>
+      </c>
+      <c r="K74" s="27"/>
+      <c r="L74" s="27"/>
+      <c r="M74" s="27"/>
+      <c r="N74" s="27"/>
+      <c r="O74" s="27"/>
+      <c r="P74" s="27"/>
+      <c r="Q74" s="27"/>
+      <c r="R74" s="27"/>
+      <c r="S74" s="27"/>
+      <c r="T74" s="27"/>
+      <c r="U74" s="27"/>
+      <c r="V74" s="27"/>
+      <c r="W74" s="27"/>
+      <c r="X74" s="27"/>
+      <c r="Y74" s="27"/>
+      <c r="Z74" s="27"/>
+      <c r="AA74" s="31"/>
+      <c r="AB74" s="27"/>
+      <c r="AC74" s="27"/>
+      <c r="AD74" s="27"/>
+      <c r="AE74" s="27"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="AR4:AU4"/>
@@ -4388,7 +4463,7 @@
     <mergeCell ref="AI5:AK5"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="L10:BD73">
+  <conditionalFormatting sqref="L10:BD74">
     <cfRule type="expression" dxfId="9" priority="50">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
add rooms to the database and make it work
</commit_message>
<xml_diff>
--- a/documentation/ESAP_Gantt_Chart.xlsx
+++ b/documentation/ESAP_Gantt_Chart.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
   <si>
     <t>Plan</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>Get recent ratings data from the backend</t>
+  </si>
+  <si>
+    <t>Calculate overall quality when reviews are added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calculate average of each ratings </t>
+  </si>
+  <si>
+    <t>Create collections for rooms and its methods</t>
   </si>
 </sst>
 </file>
@@ -949,7 +958,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1123,6 +1132,9 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1548,7 +1560,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="43"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="44"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1877,10 +1889,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BM60"/>
+  <dimension ref="A2:BM63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1918,13 +1930,13 @@
   <sheetData>
     <row r="2" spans="1:65" ht="19" customHeight="1">
       <c r="B2" s="52"/>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
       <c r="H2" s="52"/>
       <c r="I2" s="52"/>
       <c r="J2" s="36"/>
@@ -1937,7 +1949,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -1968,65 +1980,65 @@
     <row r="3" spans="1:65" ht="27" customHeight="1">
       <c r="A3" s="52"/>
       <c r="B3" s="52"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
       <c r="H3" s="52"/>
       <c r="I3" s="52"/>
       <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:65" ht="18.75" customHeight="1">
       <c r="B4" s="53"/>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="61" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
       <c r="H4" s="53"/>
       <c r="I4" s="53"/>
       <c r="J4" s="36"/>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="62">
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="63">
         <v>42660</v>
       </c>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
       <c r="T4" s="1"/>
-      <c r="AA4" s="63" t="s">
+      <c r="AA4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="63"/>
-      <c r="AD4" s="63"/>
-      <c r="AE4" s="62">
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="63">
         <v>42688</v>
       </c>
-      <c r="AF4" s="63"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
       <c r="AI4" s="28"/>
       <c r="AJ4" s="28"/>
       <c r="AK4" s="28"/>
       <c r="AN4" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="AR4" s="61">
+      <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42702</v>
-      </c>
-      <c r="AS4" s="61"/>
-      <c r="AT4" s="61"/>
-      <c r="AU4" s="61"/>
+        <v>42703</v>
+      </c>
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
       <c r="AW4" s="28"/>
       <c r="AX4" s="28"/>
       <c r="AY4" s="28"/>
@@ -2035,42 +2047,42 @@
     </row>
     <row r="5" spans="1:65">
       <c r="G5" s="1"/>
-      <c r="L5" s="63" t="s">
+      <c r="L5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="62">
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="63">
         <v>42675</v>
       </c>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="63" t="s">
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="AA5" s="63" t="s">
+      <c r="AA5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="62">
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="63">
         <v>42712</v>
       </c>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63" t="s">
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="64"/>
+      <c r="AI5" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="63"/>
+      <c r="AJ5" s="64"/>
+      <c r="AK5" s="64"/>
       <c r="AW5" s="28"/>
       <c r="AX5" s="28"/>
       <c r="AY5" s="28"/>
@@ -2993,83 +3005,83 @@
       <c r="BM20" s="51"/>
     </row>
     <row r="21" spans="1:65" ht="19" customHeight="1">
-      <c r="A21" s="17"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="D21" s="18"/>
-      <c r="E21" s="32"/>
+      <c r="E21" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F21" s="20">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G21" s="20">
         <v>1</v>
       </c>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
+      <c r="H21" s="20">
+        <v>44</v>
+      </c>
+      <c r="I21" s="20">
+        <v>1</v>
+      </c>
       <c r="J21" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="22"/>
+      <c r="L21" s="59"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="59"/>
+      <c r="P21" s="59"/>
+      <c r="Q21" s="59"/>
+      <c r="R21" s="59"/>
+      <c r="S21" s="59"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59"/>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
+      <c r="Z21" s="59"/>
       <c r="AA21" s="24"/>
-      <c r="BD21" s="51"/>
-      <c r="BE21" s="51"/>
-      <c r="BF21" s="51"/>
-      <c r="BG21" s="51"/>
-      <c r="BH21" s="51"/>
-      <c r="BI21" s="51"/>
-      <c r="BJ21" s="51"/>
-      <c r="BK21" s="51"/>
-      <c r="BL21" s="51"/>
-      <c r="BM21" s="51"/>
+      <c r="AB21" s="59"/>
+      <c r="AC21" s="59"/>
+      <c r="AD21" s="59"/>
+      <c r="AE21" s="59"/>
+      <c r="BD21" s="59"/>
+      <c r="BE21" s="59"/>
+      <c r="BF21" s="59"/>
+      <c r="BG21" s="59"/>
+      <c r="BH21" s="59"/>
+      <c r="BI21" s="59"/>
+      <c r="BJ21" s="59"/>
+      <c r="BK21" s="59"/>
+      <c r="BL21" s="59"/>
+      <c r="BM21" s="59"/>
     </row>
     <row r="22" spans="1:65" ht="19" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D22" s="18"/>
-      <c r="E22" s="32" t="s">
-        <v>61</v>
-      </c>
+      <c r="E22" s="32"/>
       <c r="F22" s="20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G22" s="20">
         <v>1</v>
       </c>
-      <c r="H22" s="20">
-        <v>12</v>
-      </c>
-      <c r="I22" s="20">
-        <v>1</v>
-      </c>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
       <c r="J22" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K22" s="22"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-      <c r="N22" s="29"/>
-      <c r="O22" s="29"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="29"/>
-      <c r="R22" s="29"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="29"/>
-      <c r="U22" s="29"/>
-      <c r="V22" s="29"/>
-      <c r="W22" s="29"/>
-      <c r="X22" s="29"/>
-      <c r="Y22" s="29"/>
-      <c r="Z22" s="29"/>
       <c r="AA22" s="24"/>
-      <c r="AB22" s="29"/>
-      <c r="AC22" s="29"/>
-      <c r="AD22" s="29"/>
-      <c r="AE22" s="29"/>
       <c r="BD22" s="51"/>
       <c r="BE22" s="51"/>
       <c r="BF22" s="51"/>
@@ -3085,24 +3097,26 @@
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="18"/>
       <c r="E23" s="32" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="F23" s="20">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G23" s="20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23" s="20">
         <v>12</v>
       </c>
-      <c r="I23" s="20"/>
+      <c r="I23" s="20">
+        <v>1</v>
+      </c>
       <c r="J23" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="22"/>
       <c r="L23" s="29"/>
@@ -3140,40 +3154,46 @@
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D24" s="18"/>
-      <c r="E24" s="32"/>
+      <c r="E24" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F24" s="20">
-        <v>1</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
+        <v>14</v>
+      </c>
+      <c r="G24" s="20">
+        <v>3</v>
+      </c>
+      <c r="H24" s="20">
+        <v>12</v>
+      </c>
       <c r="I24" s="20"/>
       <c r="J24" s="21">
         <v>0</v>
       </c>
       <c r="K24" s="22"/>
-      <c r="L24" s="48"/>
-      <c r="M24" s="48"/>
-      <c r="N24" s="48"/>
-      <c r="O24" s="48"/>
-      <c r="P24" s="48"/>
-      <c r="Q24" s="48"/>
-      <c r="R24" s="48"/>
-      <c r="S24" s="48"/>
-      <c r="T24" s="48"/>
-      <c r="U24" s="48"/>
-      <c r="V24" s="48"/>
-      <c r="W24" s="48"/>
-      <c r="X24" s="48"/>
-      <c r="Y24" s="48"/>
-      <c r="Z24" s="48"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="29"/>
+      <c r="U24" s="29"/>
+      <c r="V24" s="29"/>
+      <c r="W24" s="29"/>
+      <c r="X24" s="29"/>
+      <c r="Y24" s="29"/>
+      <c r="Z24" s="29"/>
       <c r="AA24" s="24"/>
-      <c r="AB24" s="48"/>
-      <c r="AC24" s="48"/>
-      <c r="AD24" s="48"/>
-      <c r="AE24" s="48"/>
+      <c r="AB24" s="29"/>
+      <c r="AC24" s="29"/>
+      <c r="AD24" s="29"/>
+      <c r="AE24" s="29"/>
       <c r="BD24" s="51"/>
       <c r="BE24" s="51"/>
       <c r="BF24" s="51"/>
@@ -3182,69 +3202,63 @@
       <c r="BI24" s="51"/>
       <c r="BJ24" s="51"/>
       <c r="BK24" s="51"/>
+      <c r="BL24" s="51"/>
       <c r="BM24" s="51"/>
     </row>
-    <row r="25" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A25" s="17" t="s">
+    <row r="25" spans="1:65" ht="19" customHeight="1">
+      <c r="A25" s="17"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" s="18"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="20">
+        <v>1</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="21">
+        <v>0</v>
+      </c>
+      <c r="K25" s="22"/>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="48"/>
+      <c r="P25" s="48"/>
+      <c r="Q25" s="48"/>
+      <c r="R25" s="48"/>
+      <c r="S25" s="48"/>
+      <c r="T25" s="48"/>
+      <c r="U25" s="48"/>
+      <c r="V25" s="48"/>
+      <c r="W25" s="48"/>
+      <c r="X25" s="48"/>
+      <c r="Y25" s="48"/>
+      <c r="Z25" s="48"/>
+      <c r="AA25" s="24"/>
+      <c r="AB25" s="48"/>
+      <c r="AC25" s="48"/>
+      <c r="AD25" s="48"/>
+      <c r="AE25" s="48"/>
+      <c r="BD25" s="51"/>
+      <c r="BE25" s="51"/>
+      <c r="BF25" s="51"/>
+      <c r="BG25" s="51"/>
+      <c r="BH25" s="51"/>
+      <c r="BI25" s="51"/>
+      <c r="BJ25" s="51"/>
+      <c r="BK25" s="51"/>
+      <c r="BM25" s="51"/>
+    </row>
+    <row r="26" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
+      <c r="A26" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" s="20">
-        <v>6</v>
-      </c>
-      <c r="G25" s="20">
-        <v>1</v>
-      </c>
-      <c r="H25" s="20">
-        <v>6</v>
-      </c>
-      <c r="I25" s="20">
-        <v>1</v>
-      </c>
-      <c r="J25" s="21">
-        <v>1</v>
-      </c>
-      <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
-      <c r="Q25" s="22"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-      <c r="T25" s="22"/>
-      <c r="U25" s="22"/>
-      <c r="V25" s="22"/>
-      <c r="W25" s="22"/>
-      <c r="X25" s="22"/>
-      <c r="Y25" s="22"/>
-      <c r="Z25" s="22"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="22"/>
-      <c r="AC25" s="22"/>
-      <c r="AD25" s="22"/>
-      <c r="AE25" s="22"/>
-      <c r="BD25" s="22"/>
-      <c r="BE25" s="22"/>
-      <c r="BF25" s="22"/>
-      <c r="BG25" s="22"/>
-      <c r="BH25" s="22"/>
-      <c r="BI25" s="22"/>
-      <c r="BJ25" s="22"/>
-      <c r="BK25" s="22"/>
-      <c r="BL25" s="22"/>
-      <c r="BM25" s="22"/>
-    </row>
-    <row r="26" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A26" s="17"/>
-      <c r="C26" s="19" t="s">
-        <v>51</v>
       </c>
       <c r="E26" s="32" t="s">
         <v>30</v>
@@ -3299,19 +3313,19 @@
     <row r="27" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A27" s="17"/>
       <c r="C27" s="19" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E27" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F27" s="20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G27" s="20">
         <v>1</v>
       </c>
       <c r="H27" s="20">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I27" s="20">
         <v>1</v>
@@ -3354,21 +3368,25 @@
     <row r="28" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A28" s="17"/>
       <c r="C28" s="19" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F28" s="20">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G28" s="20">
         <v>1</v>
       </c>
-      <c r="H28" s="20"/>
-      <c r="I28" s="20"/>
+      <c r="H28" s="20">
+        <v>10</v>
+      </c>
+      <c r="I28" s="20">
+        <v>1</v>
+      </c>
       <c r="J28" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="22"/>
       <c r="L28" s="22"/>
@@ -3405,14 +3423,16 @@
     <row r="29" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A29" s="17"/>
       <c r="C29" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E29" s="32"/>
+        <v>52</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F29" s="20">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G29" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
@@ -3454,25 +3474,19 @@
     <row r="30" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A30" s="17"/>
       <c r="C30" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="32" t="s">
-        <v>30</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="E30" s="32"/>
       <c r="F30" s="20">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="G30" s="20">
         <v>2</v>
       </c>
-      <c r="H30" s="20">
-        <v>31</v>
-      </c>
-      <c r="I30" s="20">
-        <v>2</v>
-      </c>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
       <c r="J30" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
@@ -3509,21 +3523,25 @@
     <row r="31" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A31" s="17"/>
       <c r="C31" s="19" t="s">
-        <v>53</v>
+        <v>117</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>61</v>
+        <v>30</v>
       </c>
       <c r="F31" s="20">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="G31" s="20">
-        <v>1</v>
-      </c>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="H31" s="20">
+        <v>31</v>
+      </c>
+      <c r="I31" s="20">
+        <v>2</v>
+      </c>
       <c r="J31" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
@@ -3560,7 +3578,7 @@
     <row r="32" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A32" s="17"/>
       <c r="C32" s="19" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="E32" s="32"/>
       <c r="F32" s="20">
@@ -3607,27 +3625,21 @@
       <c r="BM32" s="22"/>
     </row>
     <row r="33" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A33" s="17" t="s">
-        <v>75</v>
-      </c>
+      <c r="A33" s="17"/>
       <c r="C33" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E33" s="32" t="s">
-        <v>36</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="E33" s="32"/>
       <c r="F33" s="20">
         <v>11</v>
       </c>
       <c r="G33" s="20">
-        <v>2</v>
-      </c>
-      <c r="H33" s="20">
-        <v>11</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="21">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K33" s="22"/>
       <c r="L33" s="22"/>
@@ -3662,25 +3674,29 @@
       <c r="BM33" s="22"/>
     </row>
     <row r="34" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A34" s="17"/>
+      <c r="A34" s="17" t="s">
+        <v>75</v>
+      </c>
       <c r="C34" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E34" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F34" s="20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G34" s="20">
         <v>2</v>
       </c>
       <c r="H34" s="20">
-        <v>13</v>
-      </c>
-      <c r="I34" s="20"/>
+        <v>11</v>
+      </c>
+      <c r="I34" s="20">
+        <v>2</v>
+      </c>
       <c r="J34" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="22"/>
       <c r="L34" s="22"/>
@@ -3717,19 +3733,19 @@
     <row r="35" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A35" s="17"/>
       <c r="C35" s="19" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E35" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F35" s="20">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G35" s="20">
         <v>2</v>
       </c>
       <c r="H35" s="20">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="I35" s="20"/>
       <c r="J35" s="21">
@@ -3770,19 +3786,19 @@
     <row r="36" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A36" s="17"/>
       <c r="C36" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E36" s="32" t="s">
         <v>36</v>
       </c>
       <c r="F36" s="20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G36" s="20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H36" s="20">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I36" s="20"/>
       <c r="J36" s="21">
@@ -3821,29 +3837,25 @@
       <c r="BM36" s="22"/>
     </row>
     <row r="37" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A37" s="17" t="s">
-        <v>72</v>
-      </c>
+      <c r="A37" s="17"/>
       <c r="C37" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F37" s="20">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G37" s="20">
         <v>1</v>
       </c>
       <c r="H37" s="20">
-        <v>15</v>
-      </c>
-      <c r="I37" s="20">
-        <v>1</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="I37" s="20"/>
       <c r="J37" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37" s="22"/>
       <c r="L37" s="22"/>
@@ -3878,9 +3890,11 @@
       <c r="BM37" s="22"/>
     </row>
     <row r="38" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A38" s="17"/>
+      <c r="A38" s="17" t="s">
+        <v>72</v>
+      </c>
       <c r="C38" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E38" s="32" t="s">
         <v>30</v>
@@ -3935,7 +3949,7 @@
     <row r="39" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A39" s="17"/>
       <c r="C39" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E39" s="32" t="s">
         <v>30</v>
@@ -3990,7 +4004,7 @@
     <row r="40" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A40" s="17"/>
       <c r="C40" s="19" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="E40" s="32" t="s">
         <v>30</v>
@@ -3999,13 +4013,13 @@
         <v>15</v>
       </c>
       <c r="G40" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H40" s="20">
         <v>15</v>
       </c>
       <c r="I40" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" s="21">
         <v>1</v>
@@ -4045,19 +4059,25 @@
     <row r="41" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A41" s="17"/>
       <c r="C41" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E41" s="32"/>
+        <v>90</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F41" s="20">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="G41" s="20">
-        <v>1</v>
-      </c>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
+        <v>2</v>
+      </c>
+      <c r="H41" s="20">
+        <v>15</v>
+      </c>
+      <c r="I41" s="20">
+        <v>2</v>
+      </c>
       <c r="J41" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="22"/>
       <c r="L41" s="22"/>
@@ -4094,19 +4114,25 @@
     <row r="42" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A42" s="17"/>
       <c r="C42" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="E42" s="32"/>
+        <v>55</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>61</v>
+      </c>
       <c r="F42" s="20">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="G42" s="20">
-        <v>2</v>
-      </c>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
+        <v>1</v>
+      </c>
+      <c r="H42" s="20">
+        <v>35</v>
+      </c>
+      <c r="I42" s="20">
+        <v>1</v>
+      </c>
       <c r="J42" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="22"/>
       <c r="L42" s="22"/>
@@ -4143,14 +4169,14 @@
     <row r="43" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A43" s="17"/>
       <c r="C43" s="19" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="20">
         <v>1</v>
       </c>
       <c r="G43" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H43" s="20"/>
       <c r="I43" s="20"/>
@@ -4192,25 +4218,19 @@
     <row r="44" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A44" s="17"/>
       <c r="C44" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" s="32" t="s">
-        <v>61</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="E44" s="32"/>
       <c r="F44" s="20">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="G44" s="20">
-        <v>1</v>
-      </c>
-      <c r="H44" s="20">
-        <v>38</v>
-      </c>
-      <c r="I44" s="20">
-        <v>1</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H44" s="20"/>
+      <c r="I44" s="20"/>
       <c r="J44" s="21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K44" s="22"/>
       <c r="L44" s="22"/>
@@ -4247,7 +4267,7 @@
     <row r="45" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A45" s="17"/>
       <c r="C45" s="19" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E45" s="32" t="s">
         <v>61</v>
@@ -4256,13 +4276,13 @@
         <v>38</v>
       </c>
       <c r="G45" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H45" s="20">
         <v>38</v>
       </c>
       <c r="I45" s="20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" s="21">
         <v>1</v>
@@ -4302,19 +4322,19 @@
     <row r="46" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A46" s="17"/>
       <c r="C46" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="F46" s="20">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="G46" s="20">
         <v>2</v>
       </c>
       <c r="H46" s="20">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="I46" s="20">
         <v>2</v>
@@ -4357,22 +4377,22 @@
     <row r="47" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A47" s="17"/>
       <c r="C47" s="19" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E47" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F47" s="20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G47" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H47" s="20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I47" s="20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J47" s="21">
         <v>1</v>
@@ -4412,23 +4432,25 @@
     <row r="48" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A48" s="17"/>
       <c r="C48" s="19" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
       <c r="E48" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F48" s="20">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="G48" s="20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H48" s="20">
-        <v>43</v>
-      </c>
-      <c r="I48" s="20"/>
+        <v>14</v>
+      </c>
+      <c r="I48" s="20">
+        <v>3</v>
+      </c>
       <c r="J48" s="21">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="K48" s="22"/>
       <c r="L48" s="22"/>
@@ -4465,7 +4487,7 @@
     <row r="49" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A49" s="17"/>
       <c r="C49" s="19" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="E49" s="32" t="s">
         <v>30</v>
@@ -4518,26 +4540,24 @@
       <c r="BM49" s="22"/>
     </row>
     <row r="50" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A50" s="17" t="s">
-        <v>108</v>
-      </c>
+      <c r="A50" s="17"/>
       <c r="C50" s="19" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="E50" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F50" s="20">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="G50" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H50" s="20">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="I50" s="20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J50" s="21">
         <v>1</v>
@@ -4577,19 +4597,19 @@
     <row r="51" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A51" s="17"/>
       <c r="C51" s="19" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="E51" s="32" t="s">
         <v>30</v>
       </c>
       <c r="F51" s="20">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="G51" s="20">
         <v>1</v>
       </c>
       <c r="H51" s="20">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="I51" s="20">
         <v>1</v>
@@ -4632,11 +4652,13 @@
     <row r="52" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A52" s="17"/>
       <c r="C52" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="E52" s="32"/>
+        <v>119</v>
+      </c>
+      <c r="E52" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F52" s="20">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="G52" s="20">
         <v>1</v>
@@ -4679,21 +4701,29 @@
       <c r="BM52" s="22"/>
     </row>
     <row r="53" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
-      <c r="A53" s="17"/>
+      <c r="A53" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="C53" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="E53" s="32"/>
+        <v>109</v>
+      </c>
+      <c r="E53" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F53" s="20">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G53" s="20">
         <v>1</v>
       </c>
-      <c r="H53" s="20"/>
-      <c r="I53" s="20"/>
+      <c r="H53" s="20">
+        <v>28</v>
+      </c>
+      <c r="I53" s="20">
+        <v>1</v>
+      </c>
       <c r="J53" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K53" s="22"/>
       <c r="L53" s="22"/>
@@ -4729,18 +4759,26 @@
     </row>
     <row r="54" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A54" s="17"/>
-      <c r="C54" s="19"/>
-      <c r="E54" s="32"/>
+      <c r="C54" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F54" s="20">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="G54" s="20">
         <v>1</v>
       </c>
-      <c r="H54" s="20"/>
-      <c r="I54" s="20"/>
+      <c r="H54" s="20">
+        <v>28</v>
+      </c>
+      <c r="I54" s="20">
+        <v>1</v>
+      </c>
       <c r="J54" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K54" s="22"/>
       <c r="L54" s="22"/>
@@ -4776,7 +4814,9 @@
     </row>
     <row r="55" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A55" s="17"/>
-      <c r="C55" s="19"/>
+      <c r="C55" s="19" t="s">
+        <v>111</v>
+      </c>
       <c r="E55" s="32"/>
       <c r="F55" s="20">
         <v>1</v>
@@ -4823,7 +4863,9 @@
     </row>
     <row r="56" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A56" s="17"/>
-      <c r="C56" s="19"/>
+      <c r="C56" s="19" t="s">
+        <v>112</v>
+      </c>
       <c r="E56" s="32"/>
       <c r="F56" s="20">
         <v>1</v>
@@ -5056,6 +5098,147 @@
       <c r="BL60" s="22"/>
       <c r="BM60" s="22"/>
     </row>
+    <row r="61" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
+      <c r="A61" s="17"/>
+      <c r="C61" s="19"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="20">
+        <v>1</v>
+      </c>
+      <c r="G61" s="20">
+        <v>1</v>
+      </c>
+      <c r="H61" s="20"/>
+      <c r="I61" s="20"/>
+      <c r="J61" s="21">
+        <v>0</v>
+      </c>
+      <c r="K61" s="22"/>
+      <c r="L61" s="22"/>
+      <c r="M61" s="22"/>
+      <c r="N61" s="22"/>
+      <c r="O61" s="22"/>
+      <c r="P61" s="22"/>
+      <c r="Q61" s="22"/>
+      <c r="R61" s="22"/>
+      <c r="S61" s="22"/>
+      <c r="T61" s="22"/>
+      <c r="U61" s="22"/>
+      <c r="V61" s="22"/>
+      <c r="W61" s="22"/>
+      <c r="X61" s="22"/>
+      <c r="Y61" s="22"/>
+      <c r="Z61" s="22"/>
+      <c r="AA61" s="26"/>
+      <c r="AB61" s="22"/>
+      <c r="AC61" s="22"/>
+      <c r="AD61" s="22"/>
+      <c r="AE61" s="22"/>
+      <c r="BD61" s="22"/>
+      <c r="BE61" s="22"/>
+      <c r="BF61" s="22"/>
+      <c r="BG61" s="22"/>
+      <c r="BH61" s="22"/>
+      <c r="BI61" s="22"/>
+      <c r="BJ61" s="22"/>
+      <c r="BK61" s="22"/>
+      <c r="BL61" s="22"/>
+      <c r="BM61" s="22"/>
+    </row>
+    <row r="62" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
+      <c r="A62" s="17"/>
+      <c r="C62" s="19"/>
+      <c r="E62" s="32"/>
+      <c r="F62" s="20">
+        <v>1</v>
+      </c>
+      <c r="G62" s="20">
+        <v>1</v>
+      </c>
+      <c r="H62" s="20"/>
+      <c r="I62" s="20"/>
+      <c r="J62" s="21">
+        <v>0</v>
+      </c>
+      <c r="K62" s="22"/>
+      <c r="L62" s="22"/>
+      <c r="M62" s="22"/>
+      <c r="N62" s="22"/>
+      <c r="O62" s="22"/>
+      <c r="P62" s="22"/>
+      <c r="Q62" s="22"/>
+      <c r="R62" s="22"/>
+      <c r="S62" s="22"/>
+      <c r="T62" s="22"/>
+      <c r="U62" s="22"/>
+      <c r="V62" s="22"/>
+      <c r="W62" s="22"/>
+      <c r="X62" s="22"/>
+      <c r="Y62" s="22"/>
+      <c r="Z62" s="22"/>
+      <c r="AA62" s="26"/>
+      <c r="AB62" s="22"/>
+      <c r="AC62" s="22"/>
+      <c r="AD62" s="22"/>
+      <c r="AE62" s="22"/>
+      <c r="BD62" s="22"/>
+      <c r="BE62" s="22"/>
+      <c r="BF62" s="22"/>
+      <c r="BG62" s="22"/>
+      <c r="BH62" s="22"/>
+      <c r="BI62" s="22"/>
+      <c r="BJ62" s="22"/>
+      <c r="BK62" s="22"/>
+      <c r="BL62" s="22"/>
+      <c r="BM62" s="22"/>
+    </row>
+    <row r="63" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
+      <c r="A63" s="17"/>
+      <c r="C63" s="19"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="20">
+        <v>1</v>
+      </c>
+      <c r="G63" s="20">
+        <v>1</v>
+      </c>
+      <c r="H63" s="20"/>
+      <c r="I63" s="20"/>
+      <c r="J63" s="21">
+        <v>0</v>
+      </c>
+      <c r="K63" s="22"/>
+      <c r="L63" s="22"/>
+      <c r="M63" s="22"/>
+      <c r="N63" s="22"/>
+      <c r="O63" s="22"/>
+      <c r="P63" s="22"/>
+      <c r="Q63" s="22"/>
+      <c r="R63" s="22"/>
+      <c r="S63" s="22"/>
+      <c r="T63" s="22"/>
+      <c r="U63" s="22"/>
+      <c r="V63" s="22"/>
+      <c r="W63" s="22"/>
+      <c r="X63" s="22"/>
+      <c r="Y63" s="22"/>
+      <c r="Z63" s="22"/>
+      <c r="AA63" s="26"/>
+      <c r="AB63" s="22"/>
+      <c r="AC63" s="22"/>
+      <c r="AD63" s="22"/>
+      <c r="AE63" s="22"/>
+      <c r="BD63" s="22"/>
+      <c r="BE63" s="22"/>
+      <c r="BF63" s="22"/>
+      <c r="BG63" s="22"/>
+      <c r="BH63" s="22"/>
+      <c r="BI63" s="22"/>
+      <c r="BJ63" s="22"/>
+      <c r="BK63" s="22"/>
+      <c r="BL63" s="22"/>
+      <c r="BM63" s="22"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="C2:G3"/>
@@ -5073,7 +5256,7 @@
     <mergeCell ref="AI5:AK5"/>
   </mergeCells>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="L10:BL23 L25:BL60 L24:BK24 BM10:BM60">
+  <conditionalFormatting sqref="L10:BL24 L26:BL63 L25:BK25 BM10:BM63">
     <cfRule type="expression" dxfId="19" priority="50">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -5193,14 +5376,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:65" ht="19" customHeight="1">
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="60" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
       <c r="I2" s="36"/>
       <c r="J2" s="36"/>
       <c r="L2" s="37" t="s">
@@ -5212,7 +5395,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -5241,64 +5424,64 @@
       </c>
     </row>
     <row r="3" spans="1:65" ht="27" customHeight="1">
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
+      <c r="C3" s="60"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
     <row r="4" spans="1:65" ht="18.75" customHeight="1">
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
       <c r="I4" s="36"/>
       <c r="J4" s="36"/>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="63"/>
-      <c r="N4" s="63"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="62">
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="63">
         <v>42660</v>
       </c>
-      <c r="Q4" s="62"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="62"/>
+      <c r="Q4" s="63"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="63"/>
       <c r="T4" s="1"/>
-      <c r="AA4" s="63" t="s">
+      <c r="AA4" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="63"/>
-      <c r="AD4" s="63"/>
-      <c r="AE4" s="62">
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="63">
         <v>42688</v>
       </c>
-      <c r="AF4" s="63"/>
-      <c r="AG4" s="63"/>
-      <c r="AH4" s="63"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
       <c r="AI4" s="51"/>
       <c r="AJ4" s="51"/>
       <c r="AK4" s="51"/>
       <c r="AN4" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="AR4" s="61">
+      <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42702</v>
-      </c>
-      <c r="AS4" s="61"/>
-      <c r="AT4" s="61"/>
-      <c r="AU4" s="61"/>
+        <v>42703</v>
+      </c>
+      <c r="AS4" s="62"/>
+      <c r="AT4" s="62"/>
+      <c r="AU4" s="62"/>
       <c r="AW4" s="51"/>
       <c r="AX4" s="51"/>
       <c r="AY4" s="51"/>
@@ -5307,42 +5490,42 @@
     </row>
     <row r="5" spans="1:65">
       <c r="G5" s="1"/>
-      <c r="L5" s="63" t="s">
+      <c r="L5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="63"/>
-      <c r="N5" s="63"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="62">
+      <c r="M5" s="64"/>
+      <c r="N5" s="64"/>
+      <c r="O5" s="64"/>
+      <c r="P5" s="63">
         <v>42675</v>
       </c>
-      <c r="Q5" s="62"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="62"/>
-      <c r="T5" s="63" t="s">
+      <c r="Q5" s="63"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="63"/>
+      <c r="T5" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="63"/>
-      <c r="V5" s="63"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
-      <c r="AA5" s="63" t="s">
+      <c r="AA5" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="AB5" s="63"/>
-      <c r="AC5" s="63"/>
-      <c r="AD5" s="63"/>
-      <c r="AE5" s="62">
+      <c r="AB5" s="64"/>
+      <c r="AC5" s="64"/>
+      <c r="AD5" s="64"/>
+      <c r="AE5" s="63">
         <v>42712</v>
       </c>
-      <c r="AF5" s="63"/>
-      <c r="AG5" s="63"/>
-      <c r="AH5" s="63"/>
-      <c r="AI5" s="63" t="s">
+      <c r="AF5" s="64"/>
+      <c r="AG5" s="64"/>
+      <c r="AH5" s="64"/>
+      <c r="AI5" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="AJ5" s="63"/>
-      <c r="AK5" s="63"/>
+      <c r="AJ5" s="64"/>
+      <c r="AK5" s="64"/>
       <c r="AW5" s="51"/>
       <c r="AX5" s="51"/>
       <c r="AY5" s="51"/>
@@ -7240,6 +7423,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="AA4:AD4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="P5:S5"/>
@@ -7248,11 +7436,6 @@
     <mergeCell ref="AE5:AH5"/>
     <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="AE4:AH4"/>
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="AA4:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="L10:BM48">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
add a generic alert component
</commit_message>
<xml_diff>
--- a/documentation/ESAP_Gantt_Chart.xlsx
+++ b/documentation/ESAP_Gantt_Chart.xlsx
@@ -1560,7 +1560,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="44"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="45"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1891,8 +1891,8 @@
   </sheetPr>
   <dimension ref="A2:BM63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -1949,7 +1949,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42703</v>
+        <v>42704</v>
       </c>
       <c r="AS4" s="62"/>
       <c r="AT4" s="62"/>
@@ -5395,7 +5395,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -5477,7 +5477,7 @@
       </c>
       <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42703</v>
+        <v>42704</v>
       </c>
       <c r="AS4" s="62"/>
       <c r="AT4" s="62"/>
@@ -7423,11 +7423,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="AA4:AD4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="P5:S5"/>
@@ -7436,6 +7431,11 @@
     <mergeCell ref="AE5:AH5"/>
     <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="AA4:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="L10:BM48">
     <cfRule type="expression" dxfId="9" priority="2">

</xml_diff>

<commit_message>
add a few more tests.. no promises on validity of said tests :P
</commit_message>
<xml_diff>
--- a/documentation/ESAP_Gantt_Chart.xlsx
+++ b/documentation/ESAP_Gantt_Chart.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17426"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23918"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23920" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="engineering" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <definedName name="today" localSheetId="1">business!$AR$4</definedName>
     <definedName name="today">engineering!$AR$4</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
   <si>
     <t>Plan</t>
   </si>
@@ -475,7 +475,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1560,7 +1560,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="50"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="51"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1574,31 +1574,28 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>61913</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>23813</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>204788</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>14288</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1029" name="Spinner 5" descr="Period Highlight Spin Control" hidden="1">
+            <xdr:cNvPr id="1029" name="Spinner 5" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1029"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1606,12 +1603,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1629,31 +1620,28 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>61913</xdr:colOff>
+          <xdr:colOff>63500</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>23813</xdr:rowOff>
+          <xdr:rowOff>25400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>17</xdr:col>
-          <xdr:colOff>204788</xdr:colOff>
+          <xdr:colOff>203200</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>14288</xdr:rowOff>
+          <xdr:rowOff>12700</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="2049" name="Spinner 1" descr="Period Highlight Spin Control" hidden="1">
+            <xdr:cNvPr id="2049" name="Spinner 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s2049"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
           </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
+          <xdr:spPr>
             <a:xfrm>
               <a:off x="0" y="0"/>
               <a:ext cx="0" cy="0"/>
@@ -1661,12 +1649,6 @@
             <a:prstGeom prst="rect">
               <a:avLst/>
             </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData fPrintsWithSheet="0"/>
@@ -1904,49 +1886,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:BM63"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView showGridLines="0" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="48" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="7.1328125" style="28" customWidth="1"/>
-    <col min="7" max="7" width="9.796875" style="28" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1328125" style="28" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="28" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="28" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="28" customWidth="1"/>
-    <col min="10" max="10" width="7.1328125" style="47" customWidth="1"/>
-    <col min="11" max="11" width="2.796875" style="28" customWidth="1"/>
-    <col min="12" max="16" width="3.1328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.46484375" style="28" customWidth="1"/>
-    <col min="18" max="27" width="3.1328125" style="28" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="2.796875" style="28" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="2.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="43" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" style="28" customWidth="1"/>
+    <col min="12" max="16" width="3.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="28" customWidth="1"/>
+    <col min="18" max="27" width="3.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="2.83203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="43" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="56" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="56" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="2.6640625" style="1"/>
-    <col min="59" max="60" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="61" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:65" ht="19" customHeight="1">
       <c r="B2" s="52"/>
       <c r="C2" s="60" t="s">
         <v>27</v>
@@ -1967,7 +1949,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -1995,7 +1977,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:65" ht="27" customHeight="1">
       <c r="A3" s="52"/>
       <c r="B3" s="52"/>
       <c r="C3" s="60"/>
@@ -2007,7 +1989,7 @@
       <c r="I3" s="52"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:65" ht="18.75" customHeight="1">
       <c r="B4" s="53"/>
       <c r="C4" s="61" t="s">
         <v>92</v>
@@ -2052,7 +2034,7 @@
       </c>
       <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42709</v>
+        <v>42710</v>
       </c>
       <c r="AS4" s="62"/>
       <c r="AT4" s="62"/>
@@ -2063,7 +2045,7 @@
       <c r="AZ4" s="28"/>
       <c r="BA4" s="28"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:65">
       <c r="G5" s="1"/>
       <c r="L5" s="64" t="s">
         <v>13</v>
@@ -2105,7 +2087,7 @@
       <c r="AX5" s="28"/>
       <c r="AY5" s="28"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:65">
       <c r="G6" s="1"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
@@ -2124,7 +2106,7 @@
       <c r="AX6" s="28"/>
       <c r="AY6" s="28"/>
     </row>
-    <row r="7" spans="1:65" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:65" s="18" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="34"/>
@@ -2201,7 +2183,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:65" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:65" ht="13.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -2392,7 +2374,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:65" ht="15.75" customHeight="1">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="35"/>
@@ -2567,7 +2549,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:65" ht="19" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>63</v>
       </c>
@@ -2607,7 +2589,7 @@
       <c r="BL10" s="51"/>
       <c r="BM10" s="51"/>
     </row>
-    <row r="11" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:65" ht="19" customHeight="1">
       <c r="A11" s="4"/>
       <c r="C11" s="5" t="s">
         <v>37</v>
@@ -2642,7 +2624,7 @@
       <c r="BL11" s="51"/>
       <c r="BM11" s="51"/>
     </row>
-    <row r="12" spans="1:65" s="9" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:65" s="9" customFormat="1" ht="19" customHeight="1">
       <c r="A12" s="4"/>
       <c r="C12" s="5" t="s">
         <v>38</v>
@@ -2697,7 +2679,7 @@
       <c r="BL12" s="10"/>
       <c r="BM12" s="10"/>
     </row>
-    <row r="13" spans="1:65" s="9" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:65" s="9" customFormat="1" ht="19" customHeight="1">
       <c r="A13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>39</v>
@@ -2752,7 +2734,7 @@
       <c r="BL13" s="10"/>
       <c r="BM13" s="10"/>
     </row>
-    <row r="14" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:65" ht="19" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
@@ -2790,7 +2772,7 @@
       <c r="BL14" s="51"/>
       <c r="BM14" s="51"/>
     </row>
-    <row r="15" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:65" ht="19" customHeight="1">
       <c r="A15" s="17" t="s">
         <v>64</v>
       </c>
@@ -2830,7 +2812,7 @@
       <c r="BL15" s="51"/>
       <c r="BM15" s="51"/>
     </row>
-    <row r="16" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:65" ht="19" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
@@ -2868,7 +2850,7 @@
       <c r="BL16" s="51"/>
       <c r="BM16" s="51"/>
     </row>
-    <row r="17" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:65" ht="19" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19" t="s">
@@ -2906,7 +2888,7 @@
       <c r="BL17" s="51"/>
       <c r="BM17" s="51"/>
     </row>
-    <row r="18" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:65" ht="19" customHeight="1">
       <c r="A18" s="17" t="s">
         <v>65</v>
       </c>
@@ -2946,7 +2928,7 @@
       <c r="BL18" s="51"/>
       <c r="BM18" s="51"/>
     </row>
-    <row r="19" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:65" ht="19" customHeight="1">
       <c r="A19" s="17"/>
       <c r="B19" s="18"/>
       <c r="C19" s="19" t="s">
@@ -2984,7 +2966,7 @@
       <c r="BL19" s="51"/>
       <c r="BM19" s="51"/>
     </row>
-    <row r="20" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:65" ht="19" customHeight="1">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
@@ -3022,7 +3004,7 @@
       <c r="BL20" s="51"/>
       <c r="BM20" s="51"/>
     </row>
-    <row r="21" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:65" ht="19" customHeight="1">
       <c r="A21" s="18"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -3079,7 +3061,7 @@
       <c r="BL21" s="59"/>
       <c r="BM21" s="59"/>
     </row>
-    <row r="22" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:65" ht="19" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -3111,7 +3093,7 @@
       <c r="BL22" s="51"/>
       <c r="BM22" s="51"/>
     </row>
-    <row r="23" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:65" ht="19" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="18"/>
       <c r="C23" s="19" t="s">
@@ -3168,7 +3150,7 @@
       <c r="BL23" s="51"/>
       <c r="BM23" s="51"/>
     </row>
-    <row r="24" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:65" ht="19" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19" t="s">
@@ -3223,7 +3205,7 @@
       <c r="BL24" s="51"/>
       <c r="BM24" s="51"/>
     </row>
-    <row r="25" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:65" ht="19" customHeight="1">
       <c r="A25" s="17"/>
       <c r="B25" s="18"/>
       <c r="C25" s="19" t="s">
@@ -3271,7 +3253,7 @@
       <c r="BK25" s="51"/>
       <c r="BM25" s="51"/>
     </row>
-    <row r="26" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>74</v>
       </c>
@@ -3328,7 +3310,7 @@
       <c r="BL26" s="22"/>
       <c r="BM26" s="22"/>
     </row>
-    <row r="27" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A27" s="17"/>
       <c r="C27" s="19" t="s">
         <v>51</v>
@@ -3383,7 +3365,7 @@
       <c r="BL27" s="22"/>
       <c r="BM27" s="22"/>
     </row>
-    <row r="28" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A28" s="17"/>
       <c r="C28" s="19" t="s">
         <v>59</v>
@@ -3438,7 +3420,7 @@
       <c r="BL28" s="22"/>
       <c r="BM28" s="22"/>
     </row>
-    <row r="29" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A29" s="17"/>
       <c r="C29" s="19" t="s">
         <v>52</v>
@@ -3489,22 +3471,28 @@
       <c r="BL29" s="22"/>
       <c r="BM29" s="22"/>
     </row>
-    <row r="30" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A30" s="17"/>
       <c r="C30" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="32"/>
+      <c r="E30" s="32" t="s">
+        <v>30</v>
+      </c>
       <c r="F30" s="20">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="G30" s="20">
         <v>2</v>
       </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
+      <c r="H30" s="20">
+        <v>48</v>
+      </c>
+      <c r="I30" s="20">
+        <v>2</v>
+      </c>
       <c r="J30" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="22"/>
       <c r="L30" s="22"/>
@@ -3538,7 +3526,7 @@
       <c r="BL30" s="22"/>
       <c r="BM30" s="22"/>
     </row>
-    <row r="31" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A31" s="17"/>
       <c r="C31" s="19" t="s">
         <v>117</v>
@@ -3593,7 +3581,7 @@
       <c r="BL31" s="22"/>
       <c r="BM31" s="22"/>
     </row>
-    <row r="32" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A32" s="17"/>
       <c r="C32" s="19" t="s">
         <v>53</v>
@@ -3642,7 +3630,7 @@
       <c r="BL32" s="22"/>
       <c r="BM32" s="22"/>
     </row>
-    <row r="33" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A33" s="17"/>
       <c r="C33" s="19" t="s">
         <v>66</v>
@@ -3691,7 +3679,7 @@
       <c r="BL33" s="22"/>
       <c r="BM33" s="22"/>
     </row>
-    <row r="34" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A34" s="17" t="s">
         <v>75</v>
       </c>
@@ -3748,7 +3736,7 @@
       <c r="BL34" s="22"/>
       <c r="BM34" s="22"/>
     </row>
-    <row r="35" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A35" s="17"/>
       <c r="C35" s="19" t="s">
         <v>71</v>
@@ -3801,7 +3789,7 @@
       <c r="BL35" s="22"/>
       <c r="BM35" s="22"/>
     </row>
-    <row r="36" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A36" s="17"/>
       <c r="C36" s="19" t="s">
         <v>68</v>
@@ -3854,7 +3842,7 @@
       <c r="BL36" s="22"/>
       <c r="BM36" s="22"/>
     </row>
-    <row r="37" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A37" s="17"/>
       <c r="C37" s="19" t="s">
         <v>70</v>
@@ -3907,7 +3895,7 @@
       <c r="BL37" s="22"/>
       <c r="BM37" s="22"/>
     </row>
-    <row r="38" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A38" s="17" t="s">
         <v>72</v>
       </c>
@@ -3964,7 +3952,7 @@
       <c r="BL38" s="22"/>
       <c r="BM38" s="22"/>
     </row>
-    <row r="39" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A39" s="17"/>
       <c r="C39" s="19" t="s">
         <v>76</v>
@@ -4019,7 +4007,7 @@
       <c r="BL39" s="22"/>
       <c r="BM39" s="22"/>
     </row>
-    <row r="40" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A40" s="17"/>
       <c r="C40" s="19" t="s">
         <v>77</v>
@@ -4074,7 +4062,7 @@
       <c r="BL40" s="22"/>
       <c r="BM40" s="22"/>
     </row>
-    <row r="41" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A41" s="17"/>
       <c r="C41" s="19" t="s">
         <v>90</v>
@@ -4129,7 +4117,7 @@
       <c r="BL41" s="22"/>
       <c r="BM41" s="22"/>
     </row>
-    <row r="42" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A42" s="17"/>
       <c r="C42" s="19" t="s">
         <v>55</v>
@@ -4184,7 +4172,7 @@
       <c r="BL42" s="22"/>
       <c r="BM42" s="22"/>
     </row>
-    <row r="43" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A43" s="17"/>
       <c r="C43" s="19" t="s">
         <v>60</v>
@@ -4239,7 +4227,7 @@
       <c r="BL43" s="22"/>
       <c r="BM43" s="22"/>
     </row>
-    <row r="44" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A44" s="17"/>
       <c r="C44" s="19" t="s">
         <v>78</v>
@@ -4288,7 +4276,7 @@
       <c r="BL44" s="22"/>
       <c r="BM44" s="22"/>
     </row>
-    <row r="45" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A45" s="17"/>
       <c r="C45" s="19" t="s">
         <v>56</v>
@@ -4343,7 +4331,7 @@
       <c r="BL45" s="22"/>
       <c r="BM45" s="22"/>
     </row>
-    <row r="46" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A46" s="17"/>
       <c r="C46" s="19" t="s">
         <v>79</v>
@@ -4398,7 +4386,7 @@
       <c r="BL46" s="22"/>
       <c r="BM46" s="22"/>
     </row>
-    <row r="47" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A47" s="17"/>
       <c r="C47" s="19" t="s">
         <v>80</v>
@@ -4453,7 +4441,7 @@
       <c r="BL47" s="22"/>
       <c r="BM47" s="22"/>
     </row>
-    <row r="48" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A48" s="17"/>
       <c r="C48" s="19" t="s">
         <v>81</v>
@@ -4508,7 +4496,7 @@
       <c r="BL48" s="22"/>
       <c r="BM48" s="22"/>
     </row>
-    <row r="49" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A49" s="17"/>
       <c r="C49" s="19" t="s">
         <v>57</v>
@@ -4563,7 +4551,7 @@
       <c r="BL49" s="22"/>
       <c r="BM49" s="22"/>
     </row>
-    <row r="50" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A50" s="17"/>
       <c r="C50" s="19" t="s">
         <v>82</v>
@@ -4618,7 +4606,7 @@
       <c r="BL50" s="22"/>
       <c r="BM50" s="22"/>
     </row>
-    <row r="51" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A51" s="17"/>
       <c r="C51" s="19" t="s">
         <v>118</v>
@@ -4673,7 +4661,7 @@
       <c r="BL51" s="22"/>
       <c r="BM51" s="22"/>
     </row>
-    <row r="52" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A52" s="17"/>
       <c r="C52" s="19" t="s">
         <v>119</v>
@@ -4687,10 +4675,14 @@
       <c r="G52" s="20">
         <v>1</v>
       </c>
-      <c r="H52" s="20"/>
-      <c r="I52" s="20"/>
+      <c r="H52" s="20">
+        <v>50</v>
+      </c>
+      <c r="I52" s="20">
+        <v>2</v>
+      </c>
       <c r="J52" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K52" s="22"/>
       <c r="L52" s="22"/>
@@ -4724,7 +4716,7 @@
       <c r="BL52" s="22"/>
       <c r="BM52" s="22"/>
     </row>
-    <row r="53" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A53" s="17" t="s">
         <v>108</v>
       </c>
@@ -4781,7 +4773,7 @@
       <c r="BL53" s="22"/>
       <c r="BM53" s="22"/>
     </row>
-    <row r="54" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A54" s="17"/>
       <c r="C54" s="19" t="s">
         <v>110</v>
@@ -4836,7 +4828,7 @@
       <c r="BL54" s="22"/>
       <c r="BM54" s="22"/>
     </row>
-    <row r="55" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A55" s="17"/>
       <c r="C55" s="19" t="s">
         <v>111</v>
@@ -4885,7 +4877,7 @@
       <c r="BL55" s="22"/>
       <c r="BM55" s="22"/>
     </row>
-    <row r="56" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A56" s="17"/>
       <c r="C56" s="19" t="s">
         <v>112</v>
@@ -4934,7 +4926,7 @@
       <c r="BL56" s="22"/>
       <c r="BM56" s="22"/>
     </row>
-    <row r="57" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A57" s="17"/>
       <c r="C57" s="19"/>
       <c r="E57" s="32"/>
@@ -4981,7 +4973,7 @@
       <c r="BL57" s="22"/>
       <c r="BM57" s="22"/>
     </row>
-    <row r="58" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A58" s="17"/>
       <c r="C58" s="19"/>
       <c r="E58" s="32"/>
@@ -5028,7 +5020,7 @@
       <c r="BL58" s="22"/>
       <c r="BM58" s="22"/>
     </row>
-    <row r="59" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A59" s="17"/>
       <c r="C59" s="19"/>
       <c r="E59" s="32"/>
@@ -5075,7 +5067,7 @@
       <c r="BL59" s="22"/>
       <c r="BM59" s="22"/>
     </row>
-    <row r="60" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A60" s="17"/>
       <c r="C60" s="19"/>
       <c r="E60" s="32"/>
@@ -5122,7 +5114,7 @@
       <c r="BL60" s="22"/>
       <c r="BM60" s="22"/>
     </row>
-    <row r="61" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A61" s="17"/>
       <c r="C61" s="19"/>
       <c r="E61" s="32"/>
@@ -5169,7 +5161,7 @@
       <c r="BL61" s="22"/>
       <c r="BM61" s="22"/>
     </row>
-    <row r="62" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A62" s="17"/>
       <c r="C62" s="19"/>
       <c r="E62" s="32"/>
@@ -5216,7 +5208,7 @@
       <c r="BL62" s="22"/>
       <c r="BM62" s="22"/>
     </row>
-    <row r="63" spans="1:65" s="18" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:65" s="18" customFormat="1" ht="19" customHeight="1">
       <c r="A63" s="17"/>
       <c r="C63" s="19"/>
       <c r="E63" s="32"/>
@@ -5330,23 +5322,25 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>61913</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>23813</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>204788</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>14288</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5358,46 +5352,46 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:BM48"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.6640625" defaultRowHeight="16" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="48" style="46" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.1328125" style="33" customWidth="1"/>
-    <col min="6" max="6" width="7.1328125" style="51" customWidth="1"/>
-    <col min="7" max="7" width="9.796875" style="51" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.1328125" style="51" customWidth="1"/>
+    <col min="5" max="5" width="8.1640625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="7.1640625" style="51" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" style="51" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" style="51" customWidth="1"/>
-    <col min="10" max="10" width="7.1328125" style="47" customWidth="1"/>
-    <col min="11" max="11" width="2.796875" style="51" customWidth="1"/>
-    <col min="12" max="16" width="3.1328125" style="51" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="3.46484375" style="51" customWidth="1"/>
-    <col min="18" max="27" width="3.1328125" style="51" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="2.796875" style="51" bestFit="1" customWidth="1"/>
-    <col min="32" max="35" width="2.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="43" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="3.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="2.83203125" style="51" customWidth="1"/>
+    <col min="12" max="16" width="3.1640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="3.5" style="51" customWidth="1"/>
+    <col min="18" max="27" width="3.1640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="2.83203125" style="51" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="2.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="43" width="3.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="49" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="49" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="3.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="56" width="3.46484375" style="1" bestFit="1" customWidth="1"/>
+    <col min="53" max="56" width="3.5" style="1" bestFit="1" customWidth="1"/>
     <col min="57" max="16384" width="2.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:65" ht="19" customHeight="1">
       <c r="C2" s="60" t="s">
         <v>27</v>
       </c>
@@ -5417,7 +5411,7 @@
       <c r="P2" s="37"/>
       <c r="Q2" s="49">
         <f ca="1">DAYS360(P4 - 1,today) + 1</f>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R2" s="37"/>
       <c r="T2" s="38"/>
@@ -5445,7 +5439,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:65" ht="27" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:65" ht="27" customHeight="1">
       <c r="C3" s="60"/>
       <c r="D3" s="60"/>
       <c r="E3" s="60"/>
@@ -5455,7 +5449,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="36"/>
     </row>
-    <row r="4" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:65" ht="18.75" customHeight="1">
       <c r="C4" s="61" t="s">
         <v>93</v>
       </c>
@@ -5499,7 +5493,7 @@
       </c>
       <c r="AR4" s="62">
         <f ca="1">TODAY()</f>
-        <v>42709</v>
+        <v>42710</v>
       </c>
       <c r="AS4" s="62"/>
       <c r="AT4" s="62"/>
@@ -5510,7 +5504,7 @@
       <c r="AZ4" s="51"/>
       <c r="BA4" s="51"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:65">
       <c r="G5" s="1"/>
       <c r="L5" s="64" t="s">
         <v>13</v>
@@ -5552,7 +5546,7 @@
       <c r="AX5" s="51"/>
       <c r="AY5" s="51"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:65">
       <c r="G6" s="1"/>
       <c r="P6" s="50"/>
       <c r="Q6" s="50"/>
@@ -5571,7 +5565,7 @@
       <c r="AX6" s="51"/>
       <c r="AY6" s="51"/>
     </row>
-    <row r="7" spans="1:65" s="18" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:65" s="18" customFormat="1" ht="13.5" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="34"/>
@@ -5648,7 +5642,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:65" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:65" ht="13.5" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -5839,7 +5833,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:65" ht="15.75" customHeight="1">
       <c r="A9" s="18"/>
       <c r="B9" s="18"/>
       <c r="C9" s="56"/>
@@ -6014,7 +6008,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:65" ht="19" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>54</v>
       </c>
@@ -6054,7 +6048,7 @@
       <c r="BL10" s="51"/>
       <c r="BM10" s="51"/>
     </row>
-    <row r="11" spans="1:65" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:65" ht="18.75" customHeight="1">
       <c r="A11" s="17" t="s">
         <v>15</v>
       </c>
@@ -6094,7 +6088,7 @@
       <c r="BL11" s="51"/>
       <c r="BM11" s="51"/>
     </row>
-    <row r="12" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:65" ht="19" customHeight="1">
       <c r="A12" s="17"/>
       <c r="B12" s="18"/>
       <c r="C12" s="19" t="s">
@@ -6132,7 +6126,7 @@
       <c r="BL12" s="51"/>
       <c r="BM12" s="51"/>
     </row>
-    <row r="13" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:65" ht="19" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="18"/>
       <c r="C13" s="19" t="s">
@@ -6168,7 +6162,7 @@
       <c r="BL13" s="51"/>
       <c r="BM13" s="51"/>
     </row>
-    <row r="14" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:65" ht="19" customHeight="1">
       <c r="A14" s="17"/>
       <c r="B14" s="18"/>
       <c r="C14" s="19" t="s">
@@ -6204,7 +6198,7 @@
       <c r="BL14" s="51"/>
       <c r="BM14" s="51"/>
     </row>
-    <row r="15" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:65" ht="19" customHeight="1">
       <c r="A15" s="17"/>
       <c r="B15" s="18"/>
       <c r="C15" s="19" t="s">
@@ -6242,7 +6236,7 @@
       <c r="BL15" s="51"/>
       <c r="BM15" s="51"/>
     </row>
-    <row r="16" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:65" ht="19" customHeight="1">
       <c r="A16" s="17"/>
       <c r="B16" s="18"/>
       <c r="C16" s="19" t="s">
@@ -6280,7 +6274,7 @@
       <c r="BL16" s="51"/>
       <c r="BM16" s="51"/>
     </row>
-    <row r="17" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:65" ht="19" customHeight="1">
       <c r="A17" s="17"/>
       <c r="B17" s="18"/>
       <c r="C17" s="19" t="s">
@@ -6318,7 +6312,7 @@
       <c r="BL17" s="51"/>
       <c r="BM17" s="51"/>
     </row>
-    <row r="18" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:65" ht="19" customHeight="1">
       <c r="A18" s="17"/>
       <c r="B18" s="18"/>
       <c r="C18" s="19" t="s">
@@ -6356,7 +6350,7 @@
       <c r="BL18" s="51"/>
       <c r="BM18" s="51"/>
     </row>
-    <row r="19" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:65" ht="19" customHeight="1">
       <c r="A19" s="17" t="s">
         <v>88</v>
       </c>
@@ -6396,7 +6390,7 @@
       <c r="BL19" s="51"/>
       <c r="BM19" s="51"/>
     </row>
-    <row r="20" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:65" ht="19" customHeight="1">
       <c r="A20" s="17"/>
       <c r="B20" s="18"/>
       <c r="C20" s="19" t="s">
@@ -6434,7 +6428,7 @@
       <c r="BL20" s="51"/>
       <c r="BM20" s="51"/>
     </row>
-    <row r="21" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:65" ht="19" customHeight="1">
       <c r="A21" s="17"/>
       <c r="B21" s="18"/>
       <c r="C21" s="19" t="s">
@@ -6472,7 +6466,7 @@
       <c r="BL21" s="51"/>
       <c r="BM21" s="51"/>
     </row>
-    <row r="22" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:65" ht="19" customHeight="1">
       <c r="A22" s="17"/>
       <c r="B22" s="18"/>
       <c r="C22" s="19" t="s">
@@ -6510,7 +6504,7 @@
       <c r="BL22" s="51"/>
       <c r="BM22" s="51"/>
     </row>
-    <row r="23" spans="1:65" s="9" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:65" s="9" customFormat="1" ht="19" customHeight="1">
       <c r="A23" s="17"/>
       <c r="B23" s="54"/>
       <c r="C23" s="19" t="s">
@@ -6567,7 +6561,7 @@
       <c r="BL23" s="10"/>
       <c r="BM23" s="10"/>
     </row>
-    <row r="24" spans="1:65" ht="19.05" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:65" ht="19" customHeight="1">
       <c r="A24" s="17"/>
       <c r="B24" s="18"/>
       <c r="C24" s="19" t="s">
@@ -6605,7 +6599,7 @@
       <c r="BL24" s="51"/>
       <c r="BM24" s="51"/>
     </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:65">
       <c r="A25" s="17" t="s">
         <v>95</v>
       </c>
@@ -6641,7 +6635,7 @@
       <c r="BL25" s="51"/>
       <c r="BM25" s="51"/>
     </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:65">
       <c r="A26" s="17"/>
       <c r="B26" s="18"/>
       <c r="C26" s="19" t="s">
@@ -6679,7 +6673,7 @@
       <c r="BL26" s="51"/>
       <c r="BM26" s="51"/>
     </row>
-    <row r="27" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:65">
       <c r="A27" s="17"/>
       <c r="B27" s="18"/>
       <c r="C27" s="19" t="s">
@@ -6717,7 +6711,7 @@
       <c r="BL27" s="51"/>
       <c r="BM27" s="51"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:65">
       <c r="A28" s="17"/>
       <c r="B28" s="18"/>
       <c r="C28" s="19" t="s">
@@ -6755,7 +6749,7 @@
       <c r="BL28" s="51"/>
       <c r="BM28" s="51"/>
     </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:65">
       <c r="A29" s="17"/>
       <c r="B29" s="18"/>
       <c r="C29" s="19" t="s">
@@ -6812,7 +6806,7 @@
       <c r="BL29" s="58"/>
       <c r="BM29" s="58"/>
     </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:65">
       <c r="A30" s="17"/>
       <c r="B30" s="18"/>
       <c r="C30" s="19" t="s">
@@ -6869,7 +6863,7 @@
       <c r="BL30" s="58"/>
       <c r="BM30" s="58"/>
     </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:65">
       <c r="A31" s="17"/>
       <c r="B31" s="18"/>
       <c r="C31" s="19" t="s">
@@ -6926,7 +6920,7 @@
       <c r="BL31" s="58"/>
       <c r="BM31" s="58"/>
     </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:65">
       <c r="A32" s="17"/>
       <c r="B32" s="18"/>
       <c r="C32" s="19" t="s">
@@ -6964,7 +6958,7 @@
       <c r="BL32" s="51"/>
       <c r="BM32" s="51"/>
     </row>
-    <row r="33" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:65">
       <c r="A33" s="17" t="s">
         <v>101</v>
       </c>
@@ -6996,7 +6990,7 @@
       <c r="BL33" s="51"/>
       <c r="BM33" s="51"/>
     </row>
-    <row r="34" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:65">
       <c r="A34" s="17"/>
       <c r="B34" s="18"/>
       <c r="C34" s="19" t="s">
@@ -7026,7 +7020,7 @@
       <c r="BL34" s="51"/>
       <c r="BM34" s="51"/>
     </row>
-    <row r="35" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:65">
       <c r="A35" s="17"/>
       <c r="B35" s="18"/>
       <c r="C35" s="19" t="s">
@@ -7056,7 +7050,7 @@
       <c r="BL35" s="51"/>
       <c r="BM35" s="51"/>
     </row>
-    <row r="36" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:65">
       <c r="A36" s="17" t="s">
         <v>102</v>
       </c>
@@ -7088,7 +7082,7 @@
       <c r="BL36" s="51"/>
       <c r="BM36" s="51"/>
     </row>
-    <row r="37" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:65">
       <c r="A37" s="17"/>
       <c r="B37" s="18"/>
       <c r="C37" s="19" t="s">
@@ -7114,7 +7108,7 @@
       <c r="BL37" s="51"/>
       <c r="BM37" s="51"/>
     </row>
-    <row r="38" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:65">
       <c r="A38" s="17"/>
       <c r="B38" s="18"/>
       <c r="C38" s="19" t="s">
@@ -7144,7 +7138,7 @@
       <c r="BL38" s="51"/>
       <c r="BM38" s="51"/>
     </row>
-    <row r="39" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:65">
       <c r="A39" s="17"/>
       <c r="B39" s="18"/>
       <c r="C39" s="19"/>
@@ -7172,7 +7166,7 @@
       <c r="BL39" s="51"/>
       <c r="BM39" s="51"/>
     </row>
-    <row r="40" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:65">
       <c r="A40" s="17"/>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
@@ -7200,7 +7194,7 @@
       <c r="BL40" s="51"/>
       <c r="BM40" s="51"/>
     </row>
-    <row r="41" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:65">
       <c r="A41" s="17"/>
       <c r="B41" s="18"/>
       <c r="C41" s="19"/>
@@ -7228,7 +7222,7 @@
       <c r="BL41" s="51"/>
       <c r="BM41" s="51"/>
     </row>
-    <row r="42" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:65">
       <c r="A42" s="17"/>
       <c r="B42" s="18"/>
       <c r="C42" s="19"/>
@@ -7256,7 +7250,7 @@
       <c r="BL42" s="51"/>
       <c r="BM42" s="51"/>
     </row>
-    <row r="43" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:65">
       <c r="A43" s="17"/>
       <c r="B43" s="18"/>
       <c r="C43" s="19"/>
@@ -7284,7 +7278,7 @@
       <c r="BL43" s="51"/>
       <c r="BM43" s="51"/>
     </row>
-    <row r="44" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:65">
       <c r="A44" s="17"/>
       <c r="B44" s="18"/>
       <c r="C44" s="19"/>
@@ -7312,7 +7306,7 @@
       <c r="BL44" s="51"/>
       <c r="BM44" s="51"/>
     </row>
-    <row r="45" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:65">
       <c r="A45" s="17"/>
       <c r="B45" s="18"/>
       <c r="C45" s="19"/>
@@ -7340,7 +7334,7 @@
       <c r="BL45" s="51"/>
       <c r="BM45" s="51"/>
     </row>
-    <row r="46" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:65">
       <c r="A46" s="17"/>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
@@ -7368,7 +7362,7 @@
       <c r="BL46" s="51"/>
       <c r="BM46" s="51"/>
     </row>
-    <row r="47" spans="1:65" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:65">
       <c r="A47" s="17"/>
       <c r="B47" s="18"/>
       <c r="C47" s="19"/>
@@ -7396,7 +7390,7 @@
       <c r="BL47" s="51"/>
       <c r="BM47" s="51"/>
     </row>
-    <row r="48" spans="1:65" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:65" s="9" customFormat="1">
       <c r="A48" s="17"/>
       <c r="B48" s="54"/>
       <c r="C48" s="19"/>
@@ -7445,11 +7439,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="C2:H3"/>
-    <mergeCell ref="C4:H4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:S4"/>
-    <mergeCell ref="AA4:AD4"/>
     <mergeCell ref="AR4:AU4"/>
     <mergeCell ref="L5:O5"/>
     <mergeCell ref="P5:S5"/>
@@ -7458,6 +7447,11 @@
     <mergeCell ref="AE5:AH5"/>
     <mergeCell ref="AI5:AK5"/>
     <mergeCell ref="AE4:AH4"/>
+    <mergeCell ref="C2:H3"/>
+    <mergeCell ref="C4:H4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:S4"/>
+    <mergeCell ref="AA4:AD4"/>
   </mergeCells>
   <conditionalFormatting sqref="L10:BM48">
     <cfRule type="expression" dxfId="9" priority="2">
@@ -7509,23 +7503,25 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>61913</xdr:colOff>
+                    <xdr:colOff>63500</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>23813</xdr:rowOff>
+                    <xdr:rowOff>25400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>17</xdr:col>
-                    <xdr:colOff>204788</xdr:colOff>
+                    <xdr:colOff>203200</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>14288</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
             </control>
           </mc:Choice>
+          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
+    <mc:Fallback/>
   </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>